<commit_message>
remove iwo, add milkman, update stats
</commit_message>
<xml_diff>
--- a/military.xlsx
+++ b/military.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Miroslav Musarliev\Desktop\git\gitmanagedmilitaryRUC\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5AC3BC1C-A0DA-4ABD-AEC5-1D30290870A8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EB8D788D-75B0-434C-8258-32346C38F455}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{4A0BD5DB-F488-4BE9-B35B-8D149A0F13E3}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="185" uniqueCount="166">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="185" uniqueCount="165">
   <si>
     <t>deamax</t>
   </si>
@@ -438,15 +438,6 @@
     <t>19:00 - 22:00</t>
   </si>
   <si>
-    <t>iwo607</t>
-  </si>
-  <si>
-    <t>18-24pm</t>
-  </si>
-  <si>
-    <t>16:00 - 22:00</t>
-  </si>
-  <si>
     <t>did not give unit info</t>
   </si>
   <si>
@@ -523,6 +514,12 @@
   </si>
   <si>
     <t>at work, cannot give info</t>
+  </si>
+  <si>
+    <t>themilkman</t>
+  </si>
+  <si>
+    <t>did not give info</t>
   </si>
 </sst>
 </file>
@@ -973,7 +970,14 @@
   <cellStyles count="1">
     <cellStyle name="Нормален" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="2">
+  <dxfs count="3">
+    <dxf>
+      <fill>
+        <patternFill patternType="darkUp">
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <color theme="0"/>
@@ -1306,8 +1310,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{154C2D90-A5F6-425E-93A9-C4003EB71C9B}">
   <dimension ref="A1:M63"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A35" workbookViewId="0">
-      <selection activeCell="E55" sqref="E55"/>
+    <sheetView tabSelected="1" topLeftCell="A23" zoomScale="70" workbookViewId="0">
+      <selection activeCell="M43" sqref="M43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1353,7 +1357,7 @@
       <c r="K1" s="15"/>
       <c r="L1" s="23"/>
       <c r="M1" s="13" t="s">
-        <v>154</v>
+        <v>151</v>
       </c>
     </row>
     <row r="2" spans="1:13" s="22" customFormat="1" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
@@ -1465,7 +1469,7 @@
         <v>0</v>
       </c>
       <c r="J4" s="39">
-        <f t="shared" ref="J4:J64" si="0">SUM(F4:I4)</f>
+        <f t="shared" ref="J4:J46" si="0">SUM(F4:I4)</f>
         <v>280</v>
       </c>
       <c r="K4" s="38">
@@ -1912,23 +1916,23 @@
         <v>145</v>
       </c>
       <c r="G15" s="31">
-        <v>95</v>
+        <v>105</v>
       </c>
       <c r="H15" s="31">
-        <v>95</v>
+        <v>105</v>
       </c>
       <c r="I15" s="35">
         <v>0</v>
       </c>
       <c r="J15" s="39">
         <f t="shared" si="0"/>
-        <v>335</v>
+        <v>355</v>
       </c>
       <c r="K15" s="38">
         <v>5</v>
       </c>
       <c r="L15" s="26">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="M15" s="1" t="s">
         <v>39</v>
@@ -2906,51 +2910,12 @@
         <v>2</v>
       </c>
       <c r="M40" s="1" t="s">
-        <v>140</v>
-      </c>
-    </row>
-    <row r="41" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A41" s="3" t="s">
         <v>137</v>
-      </c>
-      <c r="B41" s="7">
-        <v>44442</v>
-      </c>
-      <c r="C41" s="5">
-        <v>2</v>
-      </c>
-      <c r="D41" s="9" t="s">
-        <v>138</v>
-      </c>
-      <c r="E41" s="11" t="s">
-        <v>139</v>
-      </c>
-      <c r="F41" s="32">
-        <v>125</v>
-      </c>
-      <c r="G41" s="31">
-        <v>92</v>
-      </c>
-      <c r="H41" s="31">
-        <v>60</v>
-      </c>
-      <c r="I41" s="35">
-        <v>0</v>
-      </c>
-      <c r="J41" s="40">
-        <f t="shared" si="0"/>
-        <v>277</v>
-      </c>
-      <c r="K41" s="38">
-        <v>5</v>
-      </c>
-      <c r="L41" s="26">
-        <v>4</v>
       </c>
     </row>
     <row r="42" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A42" s="3" t="s">
-        <v>141</v>
+        <v>138</v>
       </c>
       <c r="B42" s="7">
         <v>44442</v>
@@ -2959,10 +2924,10 @@
         <v>1</v>
       </c>
       <c r="D42" s="9" t="s">
-        <v>142</v>
+        <v>139</v>
       </c>
       <c r="E42" s="11" t="s">
-        <v>143</v>
+        <v>140</v>
       </c>
       <c r="F42" s="32">
         <v>112</v>
@@ -2989,22 +2954,22 @@
     </row>
     <row r="43" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A43" s="3" t="s">
-        <v>144</v>
+        <v>141</v>
       </c>
       <c r="D43" s="9" t="s">
-        <v>165</v>
+        <v>162</v>
       </c>
       <c r="J43" s="40">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="M43" s="1" t="s">
-        <v>145</v>
+        <v>142</v>
       </c>
     </row>
     <row r="44" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A44" s="3" t="s">
-        <v>146</v>
+        <v>143</v>
       </c>
       <c r="B44" s="7">
         <v>44442</v>
@@ -3013,7 +2978,7 @@
         <v>0</v>
       </c>
       <c r="D44" s="9" t="s">
-        <v>147</v>
+        <v>144</v>
       </c>
       <c r="F44" s="32">
         <v>49</v>
@@ -3043,7 +3008,7 @@
     </row>
     <row r="45" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A45" s="3" t="s">
-        <v>149</v>
+        <v>146</v>
       </c>
       <c r="B45" s="7">
         <v>44442</v>
@@ -3052,7 +3017,7 @@
         <v>7</v>
       </c>
       <c r="D45" s="9" t="s">
-        <v>150</v>
+        <v>147</v>
       </c>
       <c r="F45" s="32">
         <v>98</v>
@@ -3079,7 +3044,7 @@
     </row>
     <row r="46" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A46" s="3" t="s">
-        <v>151</v>
+        <v>148</v>
       </c>
       <c r="B46" s="7">
         <v>44442</v>
@@ -3088,7 +3053,7 @@
         <v>8</v>
       </c>
       <c r="D46" s="9" t="s">
-        <v>155</v>
+        <v>152</v>
       </c>
       <c r="F46" s="32">
         <v>96</v>
@@ -3113,23 +3078,23 @@
         <v>3</v>
       </c>
       <c r="M46" s="1" t="s">
-        <v>156</v>
+        <v>153</v>
       </c>
     </row>
     <row r="47" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A47" s="3" t="s">
-        <v>153</v>
+        <v>150</v>
       </c>
       <c r="B47" s="7">
         <v>44442</v>
       </c>
       <c r="M47" s="1" t="s">
-        <v>158</v>
+        <v>155</v>
       </c>
     </row>
     <row r="48" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A48" s="3" t="s">
-        <v>152</v>
+        <v>149</v>
       </c>
       <c r="B48" s="7">
         <v>44442</v>
@@ -3138,10 +3103,10 @@
         <v>7</v>
       </c>
       <c r="D48" s="9" t="s">
-        <v>157</v>
+        <v>154</v>
       </c>
       <c r="E48" s="14" t="s">
-        <v>159</v>
+        <v>156</v>
       </c>
       <c r="F48" s="32">
         <v>95</v>
@@ -3168,7 +3133,7 @@
     </row>
     <row r="49" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A49" s="3" t="s">
-        <v>160</v>
+        <v>157</v>
       </c>
       <c r="B49" s="7">
         <v>44442</v>
@@ -3207,7 +3172,7 @@
     </row>
     <row r="50" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A50" s="3" t="s">
-        <v>161</v>
+        <v>158</v>
       </c>
       <c r="B50" s="7">
         <v>44442</v>
@@ -3246,18 +3211,61 @@
     </row>
     <row r="51" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A51" s="3" t="s">
-        <v>162</v>
+        <v>159</v>
       </c>
       <c r="B51" s="7" t="s">
+        <v>160</v>
+      </c>
+      <c r="D51" s="9" t="s">
+        <v>161</v>
+      </c>
+      <c r="J51" s="40">
+        <f t="shared" ref="J51:J52" si="1">SUM(F51:I51)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="52" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A52" s="3" t="s">
         <v>163</v>
       </c>
-      <c r="D51" s="9" t="s">
+      <c r="B52" s="7">
+        <v>44443</v>
+      </c>
+      <c r="C52" s="5">
+        <v>9</v>
+      </c>
+      <c r="D52" s="9" t="s">
         <v>164</v>
+      </c>
+      <c r="E52" s="11" t="s">
+        <v>164</v>
+      </c>
+      <c r="F52" s="32">
+        <v>122</v>
+      </c>
+      <c r="G52" s="31">
+        <v>75</v>
+      </c>
+      <c r="H52" s="31">
+        <v>55</v>
+      </c>
+      <c r="I52" s="35">
+        <v>0</v>
+      </c>
+      <c r="J52" s="40">
+        <f t="shared" si="1"/>
+        <v>252</v>
+      </c>
+      <c r="K52" s="38">
+        <v>5</v>
+      </c>
+      <c r="L52" s="26">
+        <v>3</v>
       </c>
     </row>
     <row r="63" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A63" s="3" t="s">
-        <v>148</v>
+        <v>145</v>
       </c>
       <c r="B63" s="5">
         <f>COUNTBLANK(B3:B62)</f>
@@ -3269,12 +3277,12 @@
     <mergeCell ref="F1:I1"/>
   </mergeCells>
   <conditionalFormatting sqref="L3:L46 L48:L1048576">
-    <cfRule type="cellIs" dxfId="1" priority="6" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="2" priority="7" operator="greaterThan">
       <formula>3</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K3:K46 K48:K1048576">
-    <cfRule type="colorScale" priority="5">
+    <cfRule type="colorScale" priority="6">
       <colorScale>
         <cfvo type="num" val="2"/>
         <cfvo type="max"/>
@@ -3284,7 +3292,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F3:I46 F48:I1048576">
-    <cfRule type="colorScale" priority="4">
+    <cfRule type="colorScale" priority="5">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="max"/>
@@ -3294,7 +3302,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C1:C1048576">
-    <cfRule type="colorScale" priority="3">
+    <cfRule type="colorScale" priority="4">
       <colorScale>
         <cfvo type="num" val="-12"/>
         <cfvo type="num" val="0"/>
@@ -3306,10 +3314,10 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A1:A1048576">
-    <cfRule type="duplicateValues" dxfId="0" priority="2"/>
+    <cfRule type="duplicateValues" dxfId="1" priority="3"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="J1:J46 J48:J1048576">
-    <cfRule type="colorScale" priority="1">
+    <cfRule type="colorScale" priority="2">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="max"/>
@@ -3318,6 +3326,11 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
+  <conditionalFormatting sqref="B1:B1048576">
+    <cfRule type="containsBlanks" dxfId="0" priority="1">
+      <formula>LEN(TRIM(B1))=0</formula>
+    </cfRule>
+  </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>

</xml_diff>

<commit_message>
entered all players into list
</commit_message>
<xml_diff>
--- a/military.xlsx
+++ b/military.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Miroslav Musarliev\Desktop\git\gitmanagedmilitaryRUC\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EB8D788D-75B0-434C-8258-32346C38F455}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0E3B0EAB-6C8D-4A9C-BB4D-5333C4E3488F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{4A0BD5DB-F488-4BE9-B35B-8D149A0F13E3}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="185" uniqueCount="165">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="195" uniqueCount="175">
   <si>
     <t>deamax</t>
   </si>
@@ -261,9 +261,6 @@
     <t>11:00 - 15:00</t>
   </si>
   <si>
-    <t>DEADZONE</t>
-  </si>
-  <si>
     <t>covid</t>
   </si>
   <si>
@@ -520,6 +517,39 @@
   </si>
   <si>
     <t>did not give info</t>
+  </si>
+  <si>
+    <t>MonkeyDisco</t>
+  </si>
+  <si>
+    <t>eXeQtr</t>
+  </si>
+  <si>
+    <t>KissU</t>
+  </si>
+  <si>
+    <t>VINDICATER</t>
+  </si>
+  <si>
+    <t>dodiz</t>
+  </si>
+  <si>
+    <t>Lyne</t>
+  </si>
+  <si>
+    <t>KwEne</t>
+  </si>
+  <si>
+    <t>Zarich</t>
+  </si>
+  <si>
+    <t>DonaldDuck</t>
+  </si>
+  <si>
+    <t>Dewestator</t>
+  </si>
+  <si>
+    <t>Carbon</t>
   </si>
 </sst>
 </file>
@@ -1310,8 +1340,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{154C2D90-A5F6-425E-93A9-C4003EB71C9B}">
   <dimension ref="A1:M63"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A23" zoomScale="70" workbookViewId="0">
-      <selection activeCell="M43" sqref="M43"/>
+    <sheetView tabSelected="1" topLeftCell="A38" zoomScale="70" workbookViewId="0">
+      <selection activeCell="E64" sqref="E64"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1333,13 +1363,13 @@
   <sheetData>
     <row r="1" spans="1:13" s="13" customFormat="1" ht="122.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1" s="12" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="B1" s="12" t="s">
         <v>15</v>
       </c>
       <c r="C1" s="33" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="D1" s="12" t="s">
         <v>17</v>
@@ -1348,7 +1378,7 @@
         <v>42</v>
       </c>
       <c r="F1" s="41" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="G1" s="42"/>
       <c r="H1" s="42"/>
@@ -1357,7 +1387,7 @@
       <c r="K1" s="15"/>
       <c r="L1" s="23"/>
       <c r="M1" s="13" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
     </row>
     <row r="2" spans="1:13" s="22" customFormat="1" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
@@ -1389,10 +1419,10 @@
         <v>6</v>
       </c>
       <c r="J2" s="19" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="K2" s="36" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="L2" s="21" t="s">
         <v>44</v>
@@ -1865,7 +1895,7 @@
         <v>1</v>
       </c>
       <c r="D14" s="9" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="E14" s="11" t="s">
         <v>22</v>
@@ -1991,7 +2021,7 @@
         <v>54</v>
       </c>
       <c r="E17" s="11" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="F17" s="32">
         <v>98</v>
@@ -2181,7 +2211,7 @@
         <v>3</v>
       </c>
       <c r="M21" s="1" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
     </row>
     <row r="22" spans="1:13" x14ac:dyDescent="0.3">
@@ -2223,12 +2253,12 @@
         <v>3</v>
       </c>
       <c r="M22" s="1" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
     </row>
     <row r="23" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A23" s="3" t="s">
-        <v>78</v>
+        <v>167</v>
       </c>
       <c r="B23" s="7">
         <v>44441</v>
@@ -2237,10 +2267,10 @@
         <v>-5</v>
       </c>
       <c r="D23" s="9" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="E23" s="11" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="J23" s="39">
         <f t="shared" si="0"/>
@@ -2255,7 +2285,7 @@
     </row>
     <row r="24" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A24" s="3" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="B24" s="7">
         <v>44441</v>
@@ -2264,7 +2294,7 @@
         <v>2</v>
       </c>
       <c r="D24" s="9" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="F24" s="32">
         <v>92</v>
@@ -2291,7 +2321,7 @@
     </row>
     <row r="25" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A25" s="3" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="B25" s="7">
         <v>44441</v>
@@ -2300,10 +2330,10 @@
         <v>8</v>
       </c>
       <c r="D25" s="9" t="s">
+        <v>88</v>
+      </c>
+      <c r="E25" s="11" t="s">
         <v>89</v>
-      </c>
-      <c r="E25" s="11" t="s">
-        <v>90</v>
       </c>
       <c r="F25" s="32">
         <v>72</v>
@@ -2328,12 +2358,12 @@
         <v>3</v>
       </c>
       <c r="M25" s="1" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
     </row>
     <row r="26" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A26" s="3" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="B26" s="7">
         <v>44441</v>
@@ -2342,10 +2372,10 @@
         <v>7</v>
       </c>
       <c r="D26" s="9" t="s">
+        <v>92</v>
+      </c>
+      <c r="E26" s="11" t="s">
         <v>93</v>
-      </c>
-      <c r="E26" s="11" t="s">
-        <v>94</v>
       </c>
       <c r="F26" s="32">
         <v>98</v>
@@ -2372,7 +2402,7 @@
     </row>
     <row r="27" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A27" s="3" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="B27" s="7">
         <v>44441</v>
@@ -2381,10 +2411,10 @@
         <v>0</v>
       </c>
       <c r="D27" s="9" t="s">
+        <v>96</v>
+      </c>
+      <c r="E27" s="11" t="s">
         <v>97</v>
-      </c>
-      <c r="E27" s="11" t="s">
-        <v>98</v>
       </c>
       <c r="F27" s="32">
         <v>94</v>
@@ -2406,12 +2436,12 @@
         <v>4</v>
       </c>
       <c r="M27" s="1" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
     </row>
     <row r="28" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A28" s="3" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="B28" s="7">
         <v>44441</v>
@@ -2420,10 +2450,10 @@
         <v>7</v>
       </c>
       <c r="D28" s="9" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="E28" s="14" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="F28" s="32">
         <v>87</v>
@@ -2450,7 +2480,7 @@
     </row>
     <row r="29" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A29" s="3" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="B29" s="7">
         <v>44441</v>
@@ -2459,10 +2489,10 @@
         <v>2</v>
       </c>
       <c r="D29" s="9" t="s">
+        <v>103</v>
+      </c>
+      <c r="E29" s="11" t="s">
         <v>104</v>
-      </c>
-      <c r="E29" s="11" t="s">
-        <v>105</v>
       </c>
       <c r="F29" s="32">
         <v>116</v>
@@ -2489,7 +2519,7 @@
     </row>
     <row r="30" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A30" s="3" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="B30" s="7">
         <v>44441</v>
@@ -2498,10 +2528,10 @@
         <v>7</v>
       </c>
       <c r="D30" s="9" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="E30" s="11" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="F30" s="32">
         <v>98</v>
@@ -2528,7 +2558,7 @@
     </row>
     <row r="31" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A31" s="3" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="B31" s="7">
         <v>44441</v>
@@ -2537,10 +2567,10 @@
         <v>1</v>
       </c>
       <c r="D31" s="9" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="E31" s="11" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="F31" s="32">
         <v>66</v>
@@ -2567,13 +2597,13 @@
     </row>
     <row r="32" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A32" s="3" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="B32" s="7">
         <v>44441</v>
       </c>
       <c r="D32" s="9" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="F32" s="32">
         <v>100</v>
@@ -2597,7 +2627,7 @@
     </row>
     <row r="33" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A33" s="3" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="B33" s="7">
         <v>44441</v>
@@ -2606,10 +2636,10 @@
         <v>2</v>
       </c>
       <c r="D33" s="9" t="s">
+        <v>113</v>
+      </c>
+      <c r="E33" s="14" t="s">
         <v>114</v>
-      </c>
-      <c r="E33" s="14" t="s">
-        <v>115</v>
       </c>
       <c r="F33" s="32">
         <v>98</v>
@@ -2636,7 +2666,7 @@
     </row>
     <row r="34" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A34" s="3" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="B34" s="7">
         <v>44441</v>
@@ -2645,10 +2675,10 @@
         <v>-3</v>
       </c>
       <c r="D34" s="9" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="E34" s="11" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="F34" s="32">
         <v>95</v>
@@ -2675,7 +2705,7 @@
     </row>
     <row r="35" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A35" s="3" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="B35" s="7">
         <v>44441</v>
@@ -2684,10 +2714,10 @@
         <v>1</v>
       </c>
       <c r="D35" s="9" t="s">
+        <v>118</v>
+      </c>
+      <c r="E35" s="11" t="s">
         <v>119</v>
-      </c>
-      <c r="E35" s="11" t="s">
-        <v>120</v>
       </c>
       <c r="F35" s="32">
         <v>100</v>
@@ -2714,7 +2744,7 @@
     </row>
     <row r="36" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A36" s="3" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="B36" s="7">
         <v>44441</v>
@@ -2723,10 +2753,10 @@
         <v>0</v>
       </c>
       <c r="D36" s="9" t="s">
+        <v>121</v>
+      </c>
+      <c r="E36" s="11" t="s">
         <v>122</v>
-      </c>
-      <c r="E36" s="11" t="s">
-        <v>123</v>
       </c>
       <c r="F36" s="32">
         <v>91</v>
@@ -2753,7 +2783,7 @@
     </row>
     <row r="37" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A37" s="3" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="B37" s="7">
         <v>44442</v>
@@ -2765,7 +2795,7 @@
         <v>29</v>
       </c>
       <c r="E37" s="14" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="F37" s="32">
         <v>99</v>
@@ -2795,7 +2825,7 @@
     </row>
     <row r="38" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A38" s="3" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="B38" s="7">
         <v>44442</v>
@@ -2804,10 +2834,10 @@
         <v>1</v>
       </c>
       <c r="D38" s="9" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="E38" s="11" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="F38" s="32">
         <v>100</v>
@@ -2832,12 +2862,12 @@
         <v>3</v>
       </c>
       <c r="M38" s="1" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
     </row>
     <row r="39" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A39" s="3" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="B39" s="7">
         <v>44442</v>
@@ -2846,10 +2876,10 @@
         <v>1</v>
       </c>
       <c r="D39" s="9" t="s">
+        <v>131</v>
+      </c>
+      <c r="E39" s="11" t="s">
         <v>132</v>
-      </c>
-      <c r="E39" s="11" t="s">
-        <v>133</v>
       </c>
       <c r="F39" s="32">
         <v>155</v>
@@ -2876,7 +2906,7 @@
     </row>
     <row r="40" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A40" s="3" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="B40" s="7">
         <v>44442</v>
@@ -2885,10 +2915,10 @@
         <v>1</v>
       </c>
       <c r="D40" s="9" t="s">
+        <v>134</v>
+      </c>
+      <c r="E40" s="11" t="s">
         <v>135</v>
-      </c>
-      <c r="E40" s="11" t="s">
-        <v>136</v>
       </c>
       <c r="F40" s="32">
         <v>69</v>
@@ -2910,12 +2940,17 @@
         <v>2</v>
       </c>
       <c r="M40" s="1" t="s">
-        <v>137</v>
+        <v>136</v>
+      </c>
+    </row>
+    <row r="41" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A41" s="3" t="s">
+        <v>164</v>
       </c>
     </row>
     <row r="42" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A42" s="3" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="B42" s="7">
         <v>44442</v>
@@ -2924,10 +2959,10 @@
         <v>1</v>
       </c>
       <c r="D42" s="9" t="s">
+        <v>138</v>
+      </c>
+      <c r="E42" s="11" t="s">
         <v>139</v>
-      </c>
-      <c r="E42" s="11" t="s">
-        <v>140</v>
       </c>
       <c r="F42" s="32">
         <v>112</v>
@@ -2954,22 +2989,22 @@
     </row>
     <row r="43" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A43" s="3" t="s">
+        <v>140</v>
+      </c>
+      <c r="D43" s="9" t="s">
+        <v>161</v>
+      </c>
+      <c r="J43" s="40">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="M43" s="1" t="s">
         <v>141</v>
-      </c>
-      <c r="D43" s="9" t="s">
-        <v>162</v>
-      </c>
-      <c r="J43" s="40">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="M43" s="1" t="s">
-        <v>142</v>
       </c>
     </row>
     <row r="44" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A44" s="3" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="B44" s="7">
         <v>44442</v>
@@ -2978,7 +3013,7 @@
         <v>0</v>
       </c>
       <c r="D44" s="9" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="F44" s="32">
         <v>49</v>
@@ -3008,7 +3043,7 @@
     </row>
     <row r="45" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A45" s="3" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="B45" s="7">
         <v>44442</v>
@@ -3017,7 +3052,7 @@
         <v>7</v>
       </c>
       <c r="D45" s="9" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="F45" s="32">
         <v>98</v>
@@ -3044,7 +3079,7 @@
     </row>
     <row r="46" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A46" s="3" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="B46" s="7">
         <v>44442</v>
@@ -3053,7 +3088,7 @@
         <v>8</v>
       </c>
       <c r="D46" s="9" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="F46" s="32">
         <v>96</v>
@@ -3078,23 +3113,23 @@
         <v>3</v>
       </c>
       <c r="M46" s="1" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
     </row>
     <row r="47" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A47" s="3" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="B47" s="7">
         <v>44442</v>
       </c>
       <c r="M47" s="1" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
     </row>
     <row r="48" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A48" s="3" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="B48" s="7">
         <v>44442</v>
@@ -3103,10 +3138,10 @@
         <v>7</v>
       </c>
       <c r="D48" s="9" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="E48" s="14" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="F48" s="32">
         <v>95</v>
@@ -3133,7 +3168,7 @@
     </row>
     <row r="49" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A49" s="3" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="B49" s="7">
         <v>44442</v>
@@ -3172,7 +3207,7 @@
     </row>
     <row r="50" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A50" s="3" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="B50" s="7">
         <v>44442</v>
@@ -3211,13 +3246,13 @@
     </row>
     <row r="51" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A51" s="3" t="s">
+        <v>158</v>
+      </c>
+      <c r="B51" s="7" t="s">
         <v>159</v>
       </c>
-      <c r="B51" s="7" t="s">
+      <c r="D51" s="9" t="s">
         <v>160</v>
-      </c>
-      <c r="D51" s="9" t="s">
-        <v>161</v>
       </c>
       <c r="J51" s="40">
         <f t="shared" ref="J51:J52" si="1">SUM(F51:I51)</f>
@@ -3226,7 +3261,7 @@
     </row>
     <row r="52" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A52" s="3" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="B52" s="7">
         <v>44443</v>
@@ -3235,10 +3270,10 @@
         <v>9</v>
       </c>
       <c r="D52" s="9" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="E52" s="11" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="F52" s="32">
         <v>122</v>
@@ -3263,9 +3298,54 @@
         <v>3</v>
       </c>
     </row>
+    <row r="53" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A53" s="3" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="54" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A54" s="3" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="55" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A55" s="3" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="56" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A56" s="3" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="57" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A57" s="3" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="58" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A58" s="3" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="59" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A59" s="3" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="60" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A60" s="3" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="61" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A61" s="3" t="s">
+        <v>174</v>
+      </c>
+    </row>
     <row r="63" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A63" s="3" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="B63" s="5">
         <f>COUNTBLANK(B3:B62)</f>

</xml_diff>

<commit_message>
cleanup and sort by timezone
</commit_message>
<xml_diff>
--- a/military.xlsx
+++ b/military.xlsx
@@ -2,19 +2,23 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24326"/>
-  <workbookPr defaultThemeVersion="166925"/>
+  <workbookPr codeName="Тази_работна_книга" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Miroslav Musarliev\Desktop\git\gitmanagedmilitaryRUC\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0E3B0EAB-6C8D-4A9C-BB4D-5333C4E3488F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8F5B1E7E-D9AA-4830-AAB7-F02CA30627A6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{4A0BD5DB-F488-4BE9-B35B-8D149A0F13E3}"/>
   </bookViews>
   <sheets>
     <sheet name="Лист1" sheetId="1" r:id="rId1"/>
+    <sheet name="Лист2" sheetId="2" r:id="rId2"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Лист1!$A$2:$M$62</definedName>
+  </definedNames>
   <calcPr calcId="181029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -459,9 +463,6 @@
     <t>at work</t>
   </si>
   <si>
-    <t>Left to submit info:</t>
-  </si>
-  <si>
     <t>Udinn</t>
   </si>
   <si>
@@ -543,20 +544,23 @@
     <t>Zarich</t>
   </si>
   <si>
-    <t>DonaldDuck</t>
-  </si>
-  <si>
     <t>Dewestator</t>
   </si>
   <si>
     <t>Carbon</t>
+  </si>
+  <si>
+    <t>Left to submit:</t>
+  </si>
+  <si>
+    <t>1stWULF</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -590,6 +594,16 @@
       <charset val="204"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <i/>
+      <sz val="14"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="204"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="3">
     <fill>
@@ -605,7 +619,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="20">
+  <borders count="26">
     <border>
       <left/>
       <right/>
@@ -868,11 +882,97 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thick">
+        <color auto="1"/>
+      </left>
+      <right style="medium">
+        <color auto="1"/>
+      </right>
+      <top style="hair">
+        <color auto="1"/>
+      </top>
+      <bottom style="thick">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color auto="1"/>
+      </left>
+      <right style="medium">
+        <color auto="1"/>
+      </right>
+      <top style="hair">
+        <color auto="1"/>
+      </top>
+      <bottom style="thick">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color auto="1"/>
+      </left>
+      <right/>
+      <top style="hair">
+        <color auto="1"/>
+      </top>
+      <bottom style="thick">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color auto="1"/>
+      </right>
+      <top style="hair">
+        <color auto="1"/>
+      </top>
+      <bottom style="thick">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thick">
+        <color auto="1"/>
+      </left>
+      <right style="thick">
+        <color auto="1"/>
+      </right>
+      <top style="hair">
+        <color auto="1"/>
+      </top>
+      <bottom style="thick">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color auto="1"/>
+      </left>
+      <right style="thick">
+        <color auto="1"/>
+      </right>
+      <top style="hair">
+        <color auto="1"/>
+      </top>
+      <bottom style="thick">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="43">
+  <cellXfs count="58">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
@@ -953,9 +1053,6 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="1" fontId="2" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -996,11 +1093,145 @@
     <xf numFmtId="49" fontId="2" fillId="0" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="1" fontId="2" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="20" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="21" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="21" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="22" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="2" fillId="0" borderId="23" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="2" fillId="0" borderId="21" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="2" fillId="0" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="1" fontId="1" fillId="0" borderId="23" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="2" fillId="0" borderId="25" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="4" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="4" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Нормален" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="3">
+  <dxfs count="13">
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="lightDown">
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="2"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF0070C0"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="lightDown">
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="2"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF0070C0"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="lightDown">
+          <bgColor theme="7" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="darkUp">
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="2"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF0070C0"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <fill>
         <patternFill patternType="darkUp">
@@ -1338,10 +1569,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{154C2D90-A5F6-425E-93A9-C4003EB71C9B}">
+  <sheetPr codeName="Лист1"/>
   <dimension ref="A1:M63"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A38" zoomScale="70" workbookViewId="0">
-      <selection activeCell="E64" sqref="E64"/>
+    <sheetView tabSelected="1" topLeftCell="A31" zoomScale="70" workbookViewId="0">
+      <selection activeCell="A60" sqref="A60"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1351,11 +1583,11 @@
     <col min="3" max="3" width="7.5546875" style="5" customWidth="1"/>
     <col min="4" max="4" width="22.77734375" style="9" customWidth="1"/>
     <col min="5" max="5" width="29.33203125" style="11" customWidth="1"/>
-    <col min="6" max="6" width="6.77734375" style="32" customWidth="1"/>
-    <col min="7" max="8" width="6.77734375" style="31" customWidth="1"/>
-    <col min="9" max="9" width="6.77734375" style="35" customWidth="1"/>
-    <col min="10" max="10" width="8.88671875" style="40"/>
-    <col min="11" max="11" width="10.109375" style="38" customWidth="1"/>
+    <col min="6" max="6" width="6.77734375" style="31" customWidth="1"/>
+    <col min="7" max="8" width="6.77734375" style="30" customWidth="1"/>
+    <col min="9" max="9" width="6.77734375" style="34" customWidth="1"/>
+    <col min="10" max="10" width="8.88671875" style="39"/>
+    <col min="11" max="11" width="10.109375" style="37" customWidth="1"/>
     <col min="12" max="12" width="8.88671875" style="26"/>
     <col min="13" max="13" width="51.6640625" style="1" customWidth="1"/>
     <col min="14" max="16384" width="8.88671875" style="1"/>
@@ -1368,7 +1600,7 @@
       <c r="B1" s="12" t="s">
         <v>15</v>
       </c>
-      <c r="C1" s="33" t="s">
+      <c r="C1" s="32" t="s">
         <v>82</v>
       </c>
       <c r="D1" s="12" t="s">
@@ -1377,17 +1609,17 @@
       <c r="E1" s="12" t="s">
         <v>42</v>
       </c>
-      <c r="F1" s="41" t="s">
+      <c r="F1" s="40" t="s">
         <v>83</v>
       </c>
-      <c r="G1" s="42"/>
-      <c r="H1" s="42"/>
-      <c r="I1" s="42"/>
+      <c r="G1" s="41"/>
+      <c r="H1" s="41"/>
+      <c r="I1" s="41"/>
       <c r="J1" s="23"/>
       <c r="K1" s="15"/>
       <c r="L1" s="23"/>
       <c r="M1" s="13" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
     </row>
     <row r="2" spans="1:13" s="22" customFormat="1" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
@@ -1421,7 +1653,7 @@
       <c r="J2" s="19" t="s">
         <v>84</v>
       </c>
-      <c r="K2" s="36" t="s">
+      <c r="K2" s="35" t="s">
         <v>94</v>
       </c>
       <c r="L2" s="21" t="s">
@@ -1433,292 +1665,283 @@
     </row>
     <row r="3" spans="1:13" ht="15" thickTop="1" x14ac:dyDescent="0.3">
       <c r="A3" s="2" t="s">
-        <v>0</v>
+        <v>11</v>
       </c>
       <c r="B3" s="6">
         <v>44441</v>
       </c>
       <c r="C3" s="4">
-        <v>2</v>
+        <v>-5</v>
       </c>
       <c r="D3" s="8" t="s">
-        <v>7</v>
+        <v>28</v>
       </c>
       <c r="E3" s="10" t="s">
-        <v>19</v>
+        <v>24</v>
       </c>
       <c r="F3" s="27">
-        <v>82</v>
+        <v>111</v>
       </c>
       <c r="G3" s="28">
-        <v>60</v>
-      </c>
-      <c r="H3" s="29">
-        <v>40</v>
-      </c>
-      <c r="I3" s="34">
-        <v>0</v>
-      </c>
-      <c r="J3" s="39">
+        <v>57</v>
+      </c>
+      <c r="H3" s="28">
+        <v>48</v>
+      </c>
+      <c r="I3" s="33">
+        <v>0</v>
+      </c>
+      <c r="J3" s="38">
         <f>SUM(F3:I3)</f>
-        <v>182</v>
-      </c>
-      <c r="K3" s="37">
-        <v>4</v>
-      </c>
-      <c r="L3" s="24">
-        <v>4</v>
+        <v>216</v>
+      </c>
+      <c r="K3" s="36">
+        <v>5</v>
+      </c>
+      <c r="L3" s="57">
+        <v>3</v>
+      </c>
+      <c r="M3" s="1" t="s">
+        <v>43</v>
       </c>
     </row>
     <row r="4" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A4" s="3" t="s">
-        <v>13</v>
+        <v>166</v>
       </c>
       <c r="B4" s="6">
         <v>44441</v>
       </c>
       <c r="C4" s="5">
-        <v>0</v>
+        <v>-5</v>
       </c>
       <c r="D4" s="9" t="s">
-        <v>9</v>
-      </c>
-      <c r="E4" s="14" t="s">
-        <v>20</v>
-      </c>
-      <c r="F4" s="30">
-        <v>123</v>
-      </c>
-      <c r="G4" s="31">
-        <v>90</v>
-      </c>
-      <c r="H4" s="31">
-        <v>67</v>
-      </c>
-      <c r="I4" s="35">
-        <v>0</v>
-      </c>
-      <c r="J4" s="39">
-        <f t="shared" ref="J4:J46" si="0">SUM(F4:I4)</f>
-        <v>280</v>
-      </c>
-      <c r="K4" s="38">
-        <v>5</v>
-      </c>
-      <c r="L4" s="25">
+        <v>78</v>
+      </c>
+      <c r="E4" s="11" t="s">
+        <v>78</v>
+      </c>
+      <c r="J4" s="38">
+        <f>SUM(F4:I4)</f>
+        <v>0</v>
+      </c>
+      <c r="K4" s="37">
         <v>4</v>
       </c>
       <c r="M4" s="1" t="s">
-        <v>41</v>
+        <v>68</v>
       </c>
     </row>
     <row r="5" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A5" s="3" t="s">
-        <v>14</v>
+        <v>33</v>
       </c>
       <c r="B5" s="6">
         <v>44441</v>
       </c>
       <c r="C5" s="5">
-        <v>7</v>
+        <v>-3</v>
       </c>
       <c r="D5" s="9" t="s">
-        <v>30</v>
+        <v>34</v>
       </c>
       <c r="E5" s="11" t="s">
-        <v>21</v>
-      </c>
-      <c r="F5" s="30">
+        <v>35</v>
+      </c>
+      <c r="F5" s="31">
         <v>95</v>
       </c>
-      <c r="G5" s="31">
-        <v>75</v>
-      </c>
-      <c r="H5" s="31">
-        <v>75</v>
-      </c>
-      <c r="I5" s="35">
-        <v>0</v>
-      </c>
-      <c r="J5" s="39">
-        <f t="shared" si="0"/>
-        <v>245</v>
-      </c>
-      <c r="K5" s="38">
-        <v>4</v>
-      </c>
-      <c r="L5" s="25">
+      <c r="G5" s="30">
+        <v>76</v>
+      </c>
+      <c r="H5" s="30">
+        <v>48</v>
+      </c>
+      <c r="I5" s="34">
+        <v>0</v>
+      </c>
+      <c r="J5" s="38">
+        <f>SUM(F5:I5)</f>
+        <v>219</v>
+      </c>
+      <c r="K5" s="37">
+        <v>4</v>
+      </c>
+      <c r="L5" s="26">
         <v>4</v>
       </c>
       <c r="M5" s="1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="6" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A6" s="3" t="s">
-        <v>10</v>
+        <v>115</v>
       </c>
       <c r="B6" s="6">
         <v>44441</v>
       </c>
       <c r="C6" s="5">
-        <v>8</v>
+        <v>-3</v>
       </c>
       <c r="D6" s="9" t="s">
-        <v>56</v>
+        <v>116</v>
       </c>
       <c r="E6" s="11" t="s">
-        <v>57</v>
-      </c>
-      <c r="F6" s="30">
-        <v>98</v>
-      </c>
-      <c r="G6" s="31">
-        <v>72</v>
-      </c>
-      <c r="H6" s="31">
-        <v>53</v>
-      </c>
-      <c r="I6" s="35">
-        <v>0</v>
-      </c>
-      <c r="J6" s="39">
-        <f t="shared" si="0"/>
-        <v>223</v>
-      </c>
-      <c r="K6" s="38">
-        <v>4</v>
-      </c>
-      <c r="L6" s="25">
-        <v>3</v>
-      </c>
-      <c r="M6" s="1" t="s">
-        <v>58</v>
+        <v>125</v>
+      </c>
+      <c r="F6" s="31">
+        <v>95</v>
+      </c>
+      <c r="G6" s="30">
+        <v>75</v>
+      </c>
+      <c r="H6" s="30">
+        <v>47</v>
+      </c>
+      <c r="I6" s="34">
+        <v>0</v>
+      </c>
+      <c r="J6" s="38">
+        <f>SUM(F6:I6)</f>
+        <v>217</v>
+      </c>
+      <c r="K6" s="37">
+        <v>4</v>
+      </c>
+      <c r="L6" s="26">
+        <v>2</v>
       </c>
     </row>
     <row r="7" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A7" s="3" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="B7" s="6">
         <v>44441</v>
       </c>
       <c r="C7" s="5">
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="D7" s="9" t="s">
-        <v>29</v>
-      </c>
-      <c r="E7" s="11" t="s">
-        <v>23</v>
-      </c>
-      <c r="F7" s="30">
-        <v>100</v>
-      </c>
-      <c r="G7" s="31">
-        <v>70</v>
-      </c>
-      <c r="H7" s="31">
-        <v>50</v>
-      </c>
-      <c r="I7" s="35">
-        <v>0</v>
-      </c>
-      <c r="J7" s="39">
-        <f t="shared" si="0"/>
-        <v>220</v>
-      </c>
-      <c r="K7" s="38">
-        <v>4</v>
+        <v>9</v>
+      </c>
+      <c r="E7" s="14" t="s">
+        <v>20</v>
+      </c>
+      <c r="F7" s="29">
+        <v>123</v>
+      </c>
+      <c r="G7" s="30">
+        <v>90</v>
+      </c>
+      <c r="H7" s="30">
+        <v>67</v>
+      </c>
+      <c r="I7" s="34">
+        <v>0</v>
+      </c>
+      <c r="J7" s="38">
+        <f>SUM(F7:I7)</f>
+        <v>280</v>
+      </c>
+      <c r="K7" s="37">
+        <v>5</v>
       </c>
       <c r="L7" s="25">
         <v>4</v>
+      </c>
+      <c r="M7" s="1" t="s">
+        <v>41</v>
       </c>
     </row>
     <row r="8" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A8" s="3" t="s">
-        <v>11</v>
+        <v>31</v>
       </c>
       <c r="B8" s="6">
         <v>44441</v>
       </c>
       <c r="C8" s="5">
-        <v>-5</v>
+        <v>0</v>
       </c>
       <c r="D8" s="9" t="s">
-        <v>28</v>
+        <v>32</v>
       </c>
       <c r="E8" s="11" t="s">
-        <v>24</v>
-      </c>
-      <c r="F8" s="30">
-        <v>111</v>
-      </c>
-      <c r="G8" s="31">
-        <v>57</v>
-      </c>
-      <c r="H8" s="31">
-        <v>48</v>
-      </c>
-      <c r="I8" s="35">
-        <v>0</v>
-      </c>
-      <c r="J8" s="39">
-        <f t="shared" si="0"/>
-        <v>216</v>
-      </c>
-      <c r="K8" s="38">
-        <v>5</v>
-      </c>
-      <c r="L8" s="25">
+        <v>32</v>
+      </c>
+      <c r="F8" s="31">
+        <v>88</v>
+      </c>
+      <c r="G8" s="30">
+        <v>64</v>
+      </c>
+      <c r="H8" s="30">
+        <v>47</v>
+      </c>
+      <c r="I8" s="34">
+        <v>0</v>
+      </c>
+      <c r="J8" s="38">
+        <f>SUM(F8:I8)</f>
+        <v>199</v>
+      </c>
+      <c r="K8" s="37">
+        <v>4</v>
+      </c>
+      <c r="L8" s="26">
         <v>3</v>
       </c>
       <c r="M8" s="1" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
     </row>
     <row r="9" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A9" s="3" t="s">
-        <v>25</v>
+        <v>45</v>
       </c>
       <c r="B9" s="7">
         <v>44441</v>
       </c>
       <c r="C9" s="5">
-        <v>8</v>
+        <v>0</v>
       </c>
       <c r="D9" s="9" t="s">
-        <v>27</v>
-      </c>
-      <c r="E9" s="11" t="s">
-        <v>26</v>
-      </c>
-      <c r="F9" s="32">
-        <v>95</v>
-      </c>
-      <c r="G9" s="31">
-        <v>74</v>
-      </c>
-      <c r="H9" s="31">
-        <v>54</v>
-      </c>
-      <c r="I9" s="35">
-        <v>0</v>
-      </c>
-      <c r="J9" s="39">
-        <f t="shared" si="0"/>
-        <v>223</v>
-      </c>
-      <c r="K9" s="38">
-        <v>4</v>
+        <v>46</v>
+      </c>
+      <c r="E9" s="14" t="s">
+        <v>47</v>
+      </c>
+      <c r="F9" s="31">
+        <v>100</v>
+      </c>
+      <c r="G9" s="30">
+        <v>66</v>
+      </c>
+      <c r="H9" s="30">
+        <v>47</v>
+      </c>
+      <c r="I9" s="34">
+        <v>0</v>
+      </c>
+      <c r="J9" s="38">
+        <f>SUM(F9:I9)</f>
+        <v>213</v>
+      </c>
+      <c r="K9" s="37">
+        <v>5</v>
       </c>
       <c r="L9" s="26">
         <v>3</v>
       </c>
+      <c r="M9" s="1" t="s">
+        <v>39</v>
+      </c>
     </row>
     <row r="10" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A10" s="3" t="s">
-        <v>31</v>
+        <v>95</v>
       </c>
       <c r="B10" s="7">
         <v>44441</v>
@@ -1727,116 +1950,107 @@
         <v>0</v>
       </c>
       <c r="D10" s="9" t="s">
-        <v>32</v>
+        <v>96</v>
       </c>
       <c r="E10" s="11" t="s">
-        <v>32</v>
-      </c>
-      <c r="F10" s="32">
-        <v>88</v>
-      </c>
-      <c r="G10" s="31">
-        <v>64</v>
-      </c>
-      <c r="H10" s="31">
-        <v>47</v>
-      </c>
-      <c r="I10" s="35">
-        <v>0</v>
-      </c>
-      <c r="J10" s="39">
-        <f t="shared" si="0"/>
-        <v>199</v>
-      </c>
-      <c r="K10" s="38">
-        <v>4</v>
-      </c>
-      <c r="L10" s="26">
-        <v>3</v>
+        <v>97</v>
+      </c>
+      <c r="F10" s="31">
+        <v>94</v>
+      </c>
+      <c r="G10" s="30">
+        <v>73</v>
+      </c>
+      <c r="H10" s="30">
+        <v>74</v>
+      </c>
+      <c r="I10" s="34">
+        <v>0</v>
+      </c>
+      <c r="J10" s="38">
+        <f>SUM(F10:I10)</f>
+        <v>241</v>
+      </c>
+      <c r="K10" s="37">
+        <v>4</v>
       </c>
       <c r="M10" s="1" t="s">
-        <v>39</v>
+        <v>98</v>
       </c>
     </row>
     <row r="11" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A11" s="3" t="s">
-        <v>33</v>
+        <v>120</v>
       </c>
       <c r="B11" s="7">
         <v>44441</v>
       </c>
       <c r="C11" s="5">
-        <v>-3</v>
+        <v>0</v>
       </c>
       <c r="D11" s="9" t="s">
-        <v>34</v>
+        <v>121</v>
       </c>
       <c r="E11" s="11" t="s">
-        <v>35</v>
-      </c>
-      <c r="F11" s="32">
-        <v>95</v>
-      </c>
-      <c r="G11" s="31">
-        <v>76</v>
-      </c>
-      <c r="H11" s="31">
-        <v>48</v>
-      </c>
-      <c r="I11" s="35">
-        <v>0</v>
-      </c>
-      <c r="J11" s="39">
-        <f t="shared" si="0"/>
-        <v>219</v>
-      </c>
-      <c r="K11" s="38">
+        <v>122</v>
+      </c>
+      <c r="F11" s="31">
+        <v>91</v>
+      </c>
+      <c r="G11" s="30">
+        <v>51</v>
+      </c>
+      <c r="H11" s="30">
+        <v>33</v>
+      </c>
+      <c r="I11" s="34">
+        <v>0</v>
+      </c>
+      <c r="J11" s="38">
+        <f>SUM(F11:I11)</f>
+        <v>175</v>
+      </c>
+      <c r="K11" s="37">
         <v>4</v>
       </c>
       <c r="L11" s="26">
-        <v>4</v>
-      </c>
-      <c r="M11" s="1" t="s">
-        <v>39</v>
+        <v>3</v>
       </c>
     </row>
     <row r="12" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A12" s="3" t="s">
-        <v>36</v>
+        <v>142</v>
       </c>
       <c r="B12" s="7">
-        <v>44441</v>
+        <v>44442</v>
       </c>
       <c r="C12" s="5">
-        <v>8</v>
+        <v>0</v>
       </c>
       <c r="D12" s="9" t="s">
-        <v>37</v>
-      </c>
-      <c r="E12" s="11" t="s">
-        <v>38</v>
-      </c>
-      <c r="F12" s="32">
-        <v>97</v>
-      </c>
-      <c r="G12" s="31">
-        <v>71</v>
-      </c>
-      <c r="H12" s="31">
-        <v>54</v>
-      </c>
-      <c r="I12" s="35">
-        <v>0</v>
-      </c>
-      <c r="J12" s="39">
-        <f t="shared" si="0"/>
-        <v>222</v>
-      </c>
-      <c r="K12" s="38">
-        <v>4</v>
+        <v>143</v>
+      </c>
+      <c r="F12" s="31">
+        <v>49</v>
+      </c>
+      <c r="G12" s="30">
+        <v>32</v>
+      </c>
+      <c r="H12" s="30">
+        <v>0</v>
+      </c>
+      <c r="I12" s="34">
+        <v>0</v>
+      </c>
+      <c r="J12" s="38">
+        <f>SUM(F12:I12)</f>
+        <v>81</v>
+      </c>
+      <c r="K12" s="37">
+        <v>3</v>
       </c>
       <c r="L12" s="26">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="M12" s="1" t="s">
         <v>39</v>
@@ -1844,41 +2058,41 @@
     </row>
     <row r="13" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A13" s="3" t="s">
-        <v>45</v>
+        <v>48</v>
       </c>
       <c r="B13" s="7">
         <v>44441</v>
       </c>
       <c r="C13" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D13" s="9" t="s">
-        <v>46</v>
-      </c>
-      <c r="E13" s="14" t="s">
-        <v>47</v>
-      </c>
-      <c r="F13" s="32">
+        <v>79</v>
+      </c>
+      <c r="E13" s="11" t="s">
+        <v>22</v>
+      </c>
+      <c r="F13" s="31">
         <v>100</v>
       </c>
-      <c r="G13" s="31">
-        <v>66</v>
-      </c>
-      <c r="H13" s="31">
-        <v>47</v>
-      </c>
-      <c r="I13" s="35">
-        <v>0</v>
-      </c>
-      <c r="J13" s="39">
-        <f t="shared" si="0"/>
-        <v>213</v>
-      </c>
-      <c r="K13" s="38">
-        <v>5</v>
+      <c r="G13" s="30">
+        <v>67</v>
+      </c>
+      <c r="H13" s="30">
+        <v>45</v>
+      </c>
+      <c r="I13" s="34">
+        <v>0</v>
+      </c>
+      <c r="J13" s="38">
+        <f>SUM(F13:I13)</f>
+        <v>212</v>
+      </c>
+      <c r="K13" s="37">
+        <v>4</v>
       </c>
       <c r="L13" s="26">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="M13" s="1" t="s">
         <v>39</v>
@@ -1886,7 +2100,7 @@
     </row>
     <row r="14" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A14" s="3" t="s">
-        <v>48</v>
+        <v>52</v>
       </c>
       <c r="B14" s="7">
         <v>44441</v>
@@ -1895,82 +2109,79 @@
         <v>1</v>
       </c>
       <c r="D14" s="9" t="s">
-        <v>79</v>
+        <v>72</v>
       </c>
       <c r="E14" s="11" t="s">
-        <v>22</v>
-      </c>
-      <c r="F14" s="32">
+        <v>71</v>
+      </c>
+      <c r="F14" s="31">
         <v>100</v>
       </c>
-      <c r="G14" s="31">
-        <v>67</v>
-      </c>
-      <c r="H14" s="31">
-        <v>45</v>
-      </c>
-      <c r="I14" s="35">
-        <v>0</v>
-      </c>
-      <c r="J14" s="39">
-        <f t="shared" si="0"/>
-        <v>212</v>
-      </c>
-      <c r="K14" s="38">
+      <c r="G14" s="30">
+        <v>75</v>
+      </c>
+      <c r="H14" s="30">
+        <v>75</v>
+      </c>
+      <c r="I14" s="34">
+        <v>0</v>
+      </c>
+      <c r="J14" s="38">
+        <f>SUM(F14:I14)</f>
+        <v>250</v>
+      </c>
+      <c r="K14" s="37">
         <v>4</v>
       </c>
       <c r="L14" s="26">
         <v>4</v>
-      </c>
-      <c r="M14" s="1" t="s">
-        <v>39</v>
       </c>
     </row>
     <row r="15" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A15" s="3" t="s">
-        <v>49</v>
+        <v>53</v>
       </c>
       <c r="B15" s="7">
         <v>44441</v>
       </c>
       <c r="C15" s="5">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D15" s="9" t="s">
-        <v>50</v>
+        <v>54</v>
       </c>
       <c r="E15" s="11" t="s">
-        <v>51</v>
-      </c>
-      <c r="F15" s="32">
-        <v>145</v>
-      </c>
-      <c r="G15" s="31">
-        <v>105</v>
-      </c>
-      <c r="H15" s="31">
-        <v>105</v>
-      </c>
-      <c r="I15" s="35">
-        <v>0</v>
-      </c>
-      <c r="J15" s="39">
-        <f t="shared" si="0"/>
-        <v>355</v>
-      </c>
-      <c r="K15" s="38">
-        <v>5</v>
+        <v>85</v>
+      </c>
+      <c r="F15" s="31">
+        <v>98</v>
+      </c>
+      <c r="G15" s="30">
+        <v>74</v>
+      </c>
+      <c r="H15" s="30">
+        <v>56</v>
+      </c>
+      <c r="I15" s="34">
+        <v>0</v>
+      </c>
+      <c r="J15" s="38">
+        <f>SUM(F15:I15)</f>
+        <v>228</v>
+      </c>
+      <c r="K15" s="37">
+        <v>4</v>
       </c>
       <c r="L15" s="26">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="M15" s="1" t="s">
-        <v>39</v>
+        <v>55</v>
       </c>
     </row>
     <row r="16" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A16" s="3" t="s">
-        <v>52</v>
+        <v>63</v>
       </c>
       <c r="B16" s="7">
         <v>44441</v>
@@ -1979,37 +2190,37 @@
         <v>1</v>
       </c>
       <c r="D16" s="9" t="s">
-        <v>72</v>
+        <v>64</v>
       </c>
       <c r="E16" s="11" t="s">
-        <v>71</v>
-      </c>
-      <c r="F16" s="32">
-        <v>100</v>
-      </c>
-      <c r="G16" s="31">
-        <v>75</v>
-      </c>
-      <c r="H16" s="31">
-        <v>75</v>
-      </c>
-      <c r="I16" s="35">
-        <v>0</v>
-      </c>
-      <c r="J16" s="39">
-        <f t="shared" si="0"/>
-        <v>250</v>
-      </c>
-      <c r="K16" s="38">
+        <v>65</v>
+      </c>
+      <c r="F16" s="31">
+        <v>74</v>
+      </c>
+      <c r="G16" s="30">
+        <v>74</v>
+      </c>
+      <c r="H16" s="30">
+        <v>54</v>
+      </c>
+      <c r="I16" s="34">
+        <v>0</v>
+      </c>
+      <c r="J16" s="38">
+        <f>SUM(F16:I16)</f>
+        <v>202</v>
+      </c>
+      <c r="K16" s="37">
         <v>4</v>
       </c>
       <c r="L16" s="26">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="17" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A17" s="3" t="s">
-        <v>53</v>
+        <v>67</v>
       </c>
       <c r="B17" s="7">
         <v>44441</v>
@@ -2018,82 +2229,79 @@
         <v>1</v>
       </c>
       <c r="D17" s="9" t="s">
-        <v>54</v>
+        <v>69</v>
       </c>
       <c r="E17" s="11" t="s">
-        <v>85</v>
-      </c>
-      <c r="F17" s="32">
-        <v>98</v>
-      </c>
-      <c r="G17" s="31">
-        <v>74</v>
-      </c>
-      <c r="H17" s="31">
-        <v>56</v>
-      </c>
-      <c r="I17" s="35">
-        <v>0</v>
-      </c>
-      <c r="J17" s="39">
-        <f t="shared" si="0"/>
-        <v>228</v>
-      </c>
-      <c r="K17" s="38">
+        <v>70</v>
+      </c>
+      <c r="F17" s="31">
+        <v>82</v>
+      </c>
+      <c r="G17" s="30">
+        <v>67</v>
+      </c>
+      <c r="H17" s="30">
+        <v>48</v>
+      </c>
+      <c r="I17" s="34">
+        <v>0</v>
+      </c>
+      <c r="J17" s="38">
+        <f>SUM(F17:I17)</f>
+        <v>197</v>
+      </c>
+      <c r="K17" s="37">
         <v>4</v>
       </c>
       <c r="L17" s="26">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="M17" s="1" t="s">
-        <v>55</v>
+        <v>68</v>
       </c>
     </row>
     <row r="18" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A18" s="3" t="s">
-        <v>59</v>
+        <v>107</v>
       </c>
       <c r="B18" s="7">
         <v>44441</v>
       </c>
       <c r="C18" s="5">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="D18" s="9" t="s">
-        <v>60</v>
+        <v>96</v>
       </c>
       <c r="E18" s="11" t="s">
-        <v>62</v>
-      </c>
-      <c r="F18" s="32">
-        <v>95</v>
-      </c>
-      <c r="G18" s="31">
-        <v>75</v>
-      </c>
-      <c r="H18" s="31">
-        <v>55</v>
-      </c>
-      <c r="I18" s="35">
-        <v>0</v>
-      </c>
-      <c r="J18" s="39">
-        <f t="shared" si="0"/>
-        <v>225</v>
-      </c>
-      <c r="K18" s="38">
+        <v>108</v>
+      </c>
+      <c r="F18" s="31">
+        <v>66</v>
+      </c>
+      <c r="G18" s="30">
+        <v>40</v>
+      </c>
+      <c r="H18" s="30">
+        <v>29</v>
+      </c>
+      <c r="I18" s="34">
+        <v>0</v>
+      </c>
+      <c r="J18" s="38">
+        <f>SUM(F18:I18)</f>
+        <v>135</v>
+      </c>
+      <c r="K18" s="37">
         <v>4</v>
       </c>
       <c r="L18" s="26">
-        <v>4</v>
-      </c>
-      <c r="M18" s="1" t="s">
-        <v>61</v>
+        <v>2</v>
       </c>
     </row>
     <row r="19" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A19" s="3" t="s">
-        <v>63</v>
+        <v>117</v>
       </c>
       <c r="B19" s="7">
         <v>44441</v>
@@ -2102,190 +2310,196 @@
         <v>1</v>
       </c>
       <c r="D19" s="9" t="s">
+        <v>118</v>
+      </c>
+      <c r="E19" s="11" t="s">
+        <v>119</v>
+      </c>
+      <c r="F19" s="31">
+        <v>100</v>
+      </c>
+      <c r="G19" s="30">
         <v>64</v>
       </c>
-      <c r="E19" s="11" t="s">
-        <v>65</v>
-      </c>
-      <c r="F19" s="32">
-        <v>74</v>
-      </c>
-      <c r="G19" s="31">
-        <v>74</v>
-      </c>
-      <c r="H19" s="31">
-        <v>54</v>
-      </c>
-      <c r="I19" s="35">
-        <v>0</v>
-      </c>
-      <c r="J19" s="39">
-        <f t="shared" si="0"/>
-        <v>202</v>
-      </c>
-      <c r="K19" s="38">
+      <c r="H19" s="30">
+        <v>56</v>
+      </c>
+      <c r="I19" s="34">
+        <v>0</v>
+      </c>
+      <c r="J19" s="38">
+        <f>SUM(F19:I19)</f>
+        <v>220</v>
+      </c>
+      <c r="K19" s="37">
         <v>4</v>
       </c>
       <c r="L19" s="26">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="20" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A20" s="3" t="s">
-        <v>67</v>
+        <v>127</v>
       </c>
       <c r="B20" s="7">
-        <v>44441</v>
+        <v>44442</v>
       </c>
       <c r="C20" s="5">
         <v>1</v>
       </c>
       <c r="D20" s="9" t="s">
-        <v>69</v>
+        <v>128</v>
       </c>
       <c r="E20" s="11" t="s">
-        <v>70</v>
-      </c>
-      <c r="F20" s="32">
-        <v>82</v>
-      </c>
-      <c r="G20" s="31">
-        <v>67</v>
-      </c>
-      <c r="H20" s="31">
-        <v>48</v>
-      </c>
-      <c r="I20" s="35">
-        <v>0</v>
-      </c>
-      <c r="J20" s="39">
-        <f t="shared" si="0"/>
-        <v>197</v>
-      </c>
-      <c r="K20" s="38">
+        <v>122</v>
+      </c>
+      <c r="F20" s="31">
+        <v>100</v>
+      </c>
+      <c r="G20" s="30">
+        <v>68</v>
+      </c>
+      <c r="H20" s="30">
+        <v>50</v>
+      </c>
+      <c r="I20" s="34">
+        <v>0</v>
+      </c>
+      <c r="J20" s="38">
+        <f>SUM(F20:I20)</f>
+        <v>218</v>
+      </c>
+      <c r="K20" s="37">
         <v>4</v>
       </c>
       <c r="L20" s="26">
         <v>3</v>
       </c>
       <c r="M20" s="1" t="s">
-        <v>68</v>
+        <v>129</v>
       </c>
     </row>
     <row r="21" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A21" s="3" t="s">
-        <v>73</v>
+        <v>130</v>
       </c>
       <c r="B21" s="7">
-        <v>44441</v>
+        <v>44442</v>
       </c>
       <c r="C21" s="5">
+        <v>1</v>
+      </c>
+      <c r="D21" s="9" t="s">
+        <v>131</v>
+      </c>
+      <c r="E21" s="11" t="s">
+        <v>132</v>
+      </c>
+      <c r="F21" s="31">
+        <v>155</v>
+      </c>
+      <c r="G21" s="30">
+        <v>98</v>
+      </c>
+      <c r="H21" s="30">
+        <v>93</v>
+      </c>
+      <c r="I21" s="34">
+        <v>0</v>
+      </c>
+      <c r="J21" s="38">
+        <f>SUM(F21:I21)</f>
+        <v>346</v>
+      </c>
+      <c r="K21" s="37">
         <v>5</v>
       </c>
-      <c r="D21" s="9" t="s">
-        <v>74</v>
-      </c>
-      <c r="E21" s="11" t="s">
-        <v>75</v>
-      </c>
-      <c r="F21" s="32">
-        <v>75</v>
-      </c>
-      <c r="G21" s="31">
-        <v>65</v>
-      </c>
-      <c r="H21" s="31">
-        <v>0</v>
-      </c>
-      <c r="I21" s="35">
-        <v>0</v>
-      </c>
-      <c r="J21" s="39">
-        <f t="shared" si="0"/>
-        <v>140</v>
-      </c>
-      <c r="K21" s="38">
-        <v>4</v>
-      </c>
       <c r="L21" s="26">
-        <v>3</v>
-      </c>
-      <c r="M21" s="1" t="s">
-        <v>81</v>
+        <v>4</v>
       </c>
     </row>
     <row r="22" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A22" s="3" t="s">
-        <v>76</v>
+        <v>133</v>
       </c>
       <c r="B22" s="7">
-        <v>44441</v>
+        <v>44442</v>
       </c>
       <c r="C22" s="5">
-        <v>7</v>
+        <v>1</v>
       </c>
       <c r="D22" s="9" t="s">
-        <v>64</v>
+        <v>134</v>
       </c>
       <c r="E22" s="11" t="s">
-        <v>77</v>
-      </c>
-      <c r="F22" s="32">
-        <v>101</v>
-      </c>
-      <c r="G22" s="31">
-        <v>64</v>
-      </c>
-      <c r="H22" s="31">
-        <v>49</v>
-      </c>
-      <c r="I22" s="35">
-        <v>0</v>
-      </c>
-      <c r="J22" s="39">
-        <f t="shared" si="0"/>
-        <v>214</v>
-      </c>
-      <c r="K22" s="38">
-        <v>4</v>
+        <v>135</v>
+      </c>
+      <c r="F22" s="31">
+        <v>69</v>
+      </c>
+      <c r="G22" s="30">
+        <v>68</v>
+      </c>
+      <c r="H22" s="30">
+        <v>45</v>
+      </c>
+      <c r="I22" s="34">
+        <v>0</v>
+      </c>
+      <c r="J22" s="38">
+        <f>SUM(F22:I22)</f>
+        <v>182</v>
       </c>
       <c r="L22" s="26">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="M22" s="1" t="s">
-        <v>80</v>
+        <v>136</v>
       </c>
     </row>
     <row r="23" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A23" s="3" t="s">
-        <v>167</v>
+        <v>137</v>
       </c>
       <c r="B23" s="7">
-        <v>44441</v>
+        <v>44442</v>
       </c>
       <c r="C23" s="5">
-        <v>-5</v>
+        <v>1</v>
       </c>
       <c r="D23" s="9" t="s">
-        <v>78</v>
+        <v>138</v>
       </c>
       <c r="E23" s="11" t="s">
-        <v>78</v>
-      </c>
-      <c r="J23" s="39">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="K23" s="38">
-        <v>4</v>
-      </c>
-      <c r="M23" s="1" t="s">
-        <v>68</v>
+        <v>139</v>
+      </c>
+      <c r="F23" s="31">
+        <v>120</v>
+      </c>
+      <c r="G23" s="30">
+        <v>90</v>
+      </c>
+      <c r="H23" s="30">
+        <v>56</v>
+      </c>
+      <c r="I23" s="34">
+        <v>0</v>
+      </c>
+      <c r="J23" s="38">
+        <f>SUM(F23:I23)</f>
+        <v>266</v>
+      </c>
+      <c r="K23" s="37">
+        <v>5</v>
+      </c>
+      <c r="L23" s="26">
+        <v>4</v>
       </c>
     </row>
     <row r="24" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A24" s="3" t="s">
-        <v>86</v>
+        <v>0</v>
       </c>
       <c r="B24" s="7">
         <v>44441</v>
@@ -2294,106 +2508,106 @@
         <v>2</v>
       </c>
       <c r="D24" s="9" t="s">
-        <v>111</v>
-      </c>
-      <c r="F24" s="32">
-        <v>92</v>
-      </c>
-      <c r="G24" s="31">
-        <v>70</v>
-      </c>
-      <c r="H24" s="31">
-        <v>42</v>
-      </c>
-      <c r="I24" s="35">
-        <v>0</v>
-      </c>
-      <c r="J24" s="39">
-        <f t="shared" si="0"/>
-        <v>204</v>
-      </c>
-      <c r="K24" s="38">
+        <v>7</v>
+      </c>
+      <c r="E24" s="11" t="s">
+        <v>19</v>
+      </c>
+      <c r="F24" s="29">
+        <v>82</v>
+      </c>
+      <c r="G24" s="56">
+        <v>60</v>
+      </c>
+      <c r="H24" s="30">
+        <v>40</v>
+      </c>
+      <c r="I24" s="34">
+        <v>0</v>
+      </c>
+      <c r="J24" s="38">
+        <f>SUM(F24:I24)</f>
+        <v>182</v>
+      </c>
+      <c r="K24" s="37">
         <v>4</v>
       </c>
       <c r="L24" s="26">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="25" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A25" s="3" t="s">
-        <v>87</v>
+        <v>49</v>
       </c>
       <c r="B25" s="7">
         <v>44441</v>
       </c>
       <c r="C25" s="5">
-        <v>8</v>
+        <v>2</v>
       </c>
       <c r="D25" s="9" t="s">
-        <v>88</v>
+        <v>50</v>
       </c>
       <c r="E25" s="11" t="s">
-        <v>89</v>
-      </c>
-      <c r="F25" s="32">
-        <v>72</v>
-      </c>
-      <c r="G25" s="31">
-        <v>55</v>
-      </c>
-      <c r="H25" s="31">
+        <v>51</v>
+      </c>
+      <c r="F25" s="31">
+        <v>145</v>
+      </c>
+      <c r="G25" s="30">
+        <v>105</v>
+      </c>
+      <c r="H25" s="30">
+        <v>105</v>
+      </c>
+      <c r="I25" s="34">
+        <v>0</v>
+      </c>
+      <c r="J25" s="38">
+        <f>SUM(F25:I25)</f>
+        <v>355</v>
+      </c>
+      <c r="K25" s="37">
+        <v>5</v>
+      </c>
+      <c r="L25" s="26">
+        <v>5</v>
+      </c>
+      <c r="M25" s="1" t="s">
         <v>39</v>
-      </c>
-      <c r="I25" s="35">
-        <v>0</v>
-      </c>
-      <c r="J25" s="39">
-        <f t="shared" si="0"/>
-        <v>166</v>
-      </c>
-      <c r="K25" s="38">
-        <v>4</v>
-      </c>
-      <c r="L25" s="26">
-        <v>3</v>
-      </c>
-      <c r="M25" s="1" t="s">
-        <v>90</v>
       </c>
     </row>
     <row r="26" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A26" s="3" t="s">
-        <v>91</v>
+        <v>86</v>
       </c>
       <c r="B26" s="7">
         <v>44441</v>
       </c>
       <c r="C26" s="5">
-        <v>7</v>
+        <v>2</v>
       </c>
       <c r="D26" s="9" t="s">
+        <v>111</v>
+      </c>
+      <c r="F26" s="31">
         <v>92</v>
       </c>
-      <c r="E26" s="11" t="s">
-        <v>93</v>
-      </c>
-      <c r="F26" s="32">
-        <v>98</v>
-      </c>
-      <c r="G26" s="31">
-        <v>63</v>
-      </c>
-      <c r="H26" s="31">
-        <v>0</v>
-      </c>
-      <c r="I26" s="35">
-        <v>0</v>
-      </c>
-      <c r="J26" s="39">
-        <f t="shared" si="0"/>
-        <v>161</v>
-      </c>
-      <c r="K26" s="38">
+      <c r="G26" s="30">
+        <v>70</v>
+      </c>
+      <c r="H26" s="30">
+        <v>42</v>
+      </c>
+      <c r="I26" s="34">
+        <v>0</v>
+      </c>
+      <c r="J26" s="38">
+        <f>SUM(F26:I26)</f>
+        <v>204</v>
+      </c>
+      <c r="K26" s="37">
         <v>4</v>
       </c>
       <c r="L26" s="26">
@@ -2402,76 +2616,76 @@
     </row>
     <row r="27" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A27" s="3" t="s">
-        <v>95</v>
+        <v>102</v>
       </c>
       <c r="B27" s="7">
         <v>44441</v>
       </c>
       <c r="C27" s="5">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="D27" s="9" t="s">
-        <v>96</v>
+        <v>103</v>
       </c>
       <c r="E27" s="11" t="s">
-        <v>97</v>
-      </c>
-      <c r="F27" s="32">
-        <v>94</v>
-      </c>
-      <c r="G27" s="31">
-        <v>73</v>
-      </c>
-      <c r="H27" s="31">
-        <v>74</v>
-      </c>
-      <c r="I27" s="35">
-        <v>0</v>
-      </c>
-      <c r="J27" s="40">
-        <f t="shared" si="0"/>
-        <v>241</v>
-      </c>
-      <c r="K27" s="38">
-        <v>4</v>
-      </c>
-      <c r="M27" s="1" t="s">
-        <v>98</v>
+        <v>104</v>
+      </c>
+      <c r="F27" s="31">
+        <v>116</v>
+      </c>
+      <c r="G27" s="30">
+        <v>93</v>
+      </c>
+      <c r="H27" s="30">
+        <v>61</v>
+      </c>
+      <c r="I27" s="34">
+        <v>0</v>
+      </c>
+      <c r="J27" s="39">
+        <f>SUM(F27:I27)</f>
+        <v>270</v>
+      </c>
+      <c r="K27" s="37">
+        <v>5</v>
+      </c>
+      <c r="L27" s="26">
+        <v>3</v>
       </c>
     </row>
     <row r="28" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A28" s="3" t="s">
-        <v>99</v>
+        <v>112</v>
       </c>
       <c r="B28" s="7">
         <v>44441</v>
       </c>
       <c r="C28" s="5">
-        <v>7</v>
+        <v>2</v>
       </c>
       <c r="D28" s="9" t="s">
-        <v>101</v>
+        <v>113</v>
       </c>
       <c r="E28" s="14" t="s">
-        <v>100</v>
-      </c>
-      <c r="F28" s="32">
-        <v>87</v>
-      </c>
-      <c r="G28" s="31">
-        <v>65</v>
-      </c>
-      <c r="H28" s="31">
-        <v>48</v>
-      </c>
-      <c r="I28" s="35">
-        <v>0</v>
-      </c>
-      <c r="J28" s="40">
-        <f t="shared" si="0"/>
-        <v>200</v>
-      </c>
-      <c r="K28" s="38">
+        <v>114</v>
+      </c>
+      <c r="F28" s="31">
+        <v>98</v>
+      </c>
+      <c r="G28" s="30">
+        <v>69</v>
+      </c>
+      <c r="H28" s="30">
+        <v>49</v>
+      </c>
+      <c r="I28" s="34">
+        <v>0</v>
+      </c>
+      <c r="J28" s="39">
+        <f>SUM(F28:I28)</f>
+        <v>216</v>
+      </c>
+      <c r="K28" s="37">
         <v>4</v>
       </c>
       <c r="L28" s="26">
@@ -2480,597 +2694,682 @@
     </row>
     <row r="29" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A29" s="3" t="s">
-        <v>102</v>
+        <v>123</v>
       </c>
       <c r="B29" s="7">
-        <v>44441</v>
+        <v>44442</v>
       </c>
       <c r="C29" s="5">
         <v>2</v>
       </c>
       <c r="D29" s="9" t="s">
-        <v>103</v>
-      </c>
-      <c r="E29" s="11" t="s">
-        <v>104</v>
-      </c>
-      <c r="F29" s="32">
-        <v>116</v>
-      </c>
-      <c r="G29" s="31">
-        <v>93</v>
-      </c>
-      <c r="H29" s="31">
-        <v>61</v>
-      </c>
-      <c r="I29" s="35">
-        <v>0</v>
-      </c>
-      <c r="J29" s="40">
-        <f t="shared" si="0"/>
-        <v>270</v>
-      </c>
-      <c r="K29" s="38">
+        <v>29</v>
+      </c>
+      <c r="E29" s="14" t="s">
+        <v>124</v>
+      </c>
+      <c r="F29" s="31">
+        <v>99</v>
+      </c>
+      <c r="G29" s="30">
+        <v>82</v>
+      </c>
+      <c r="H29" s="30">
+        <v>55</v>
+      </c>
+      <c r="I29" s="34">
+        <v>0</v>
+      </c>
+      <c r="J29" s="39">
+        <f>SUM(F29:I29)</f>
+        <v>236</v>
+      </c>
+      <c r="K29" s="37">
         <v>5</v>
       </c>
       <c r="L29" s="26">
-        <v>3</v>
+        <v>4</v>
+      </c>
+      <c r="M29" s="1" t="s">
+        <v>39</v>
       </c>
     </row>
     <row r="30" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A30" s="3" t="s">
-        <v>105</v>
+        <v>59</v>
       </c>
       <c r="B30" s="7">
         <v>44441</v>
       </c>
       <c r="C30" s="5">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="D30" s="9" t="s">
-        <v>106</v>
+        <v>60</v>
       </c>
       <c r="E30" s="11" t="s">
-        <v>93</v>
-      </c>
-      <c r="F30" s="32">
-        <v>98</v>
-      </c>
-      <c r="G30" s="31">
-        <v>66</v>
-      </c>
-      <c r="H30" s="31">
-        <v>58</v>
-      </c>
-      <c r="I30" s="35">
-        <v>0</v>
-      </c>
-      <c r="J30" s="40">
-        <f t="shared" si="0"/>
-        <v>222</v>
-      </c>
-      <c r="K30" s="38">
+        <v>62</v>
+      </c>
+      <c r="F30" s="31">
+        <v>95</v>
+      </c>
+      <c r="G30" s="30">
+        <v>75</v>
+      </c>
+      <c r="H30" s="30">
+        <v>55</v>
+      </c>
+      <c r="I30" s="34">
+        <v>0</v>
+      </c>
+      <c r="J30" s="39">
+        <f>SUM(F30:I30)</f>
+        <v>225</v>
+      </c>
+      <c r="K30" s="37">
         <v>4</v>
       </c>
       <c r="L30" s="26">
         <v>4</v>
+      </c>
+      <c r="M30" s="1" t="s">
+        <v>61</v>
       </c>
     </row>
     <row r="31" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A31" s="3" t="s">
-        <v>107</v>
+        <v>73</v>
       </c>
       <c r="B31" s="7">
         <v>44441</v>
       </c>
       <c r="C31" s="5">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="D31" s="9" t="s">
-        <v>96</v>
+        <v>74</v>
       </c>
       <c r="E31" s="11" t="s">
-        <v>108</v>
-      </c>
-      <c r="F31" s="32">
-        <v>66</v>
-      </c>
-      <c r="G31" s="31">
-        <v>40</v>
-      </c>
-      <c r="H31" s="31">
-        <v>29</v>
-      </c>
-      <c r="I31" s="35">
-        <v>0</v>
-      </c>
-      <c r="J31" s="40">
-        <f t="shared" si="0"/>
-        <v>135</v>
-      </c>
-      <c r="K31" s="38">
+        <v>75</v>
+      </c>
+      <c r="F31" s="31">
+        <v>75</v>
+      </c>
+      <c r="G31" s="30">
+        <v>65</v>
+      </c>
+      <c r="H31" s="30">
+        <v>0</v>
+      </c>
+      <c r="I31" s="34">
+        <v>0</v>
+      </c>
+      <c r="J31" s="39">
+        <f>SUM(F31:I31)</f>
+        <v>140</v>
+      </c>
+      <c r="K31" s="37">
         <v>4</v>
       </c>
       <c r="L31" s="26">
-        <v>2</v>
+        <v>3</v>
+      </c>
+      <c r="M31" s="1" t="s">
+        <v>81</v>
       </c>
     </row>
     <row r="32" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A32" s="3" t="s">
-        <v>110</v>
+        <v>14</v>
       </c>
       <c r="B32" s="7">
         <v>44441</v>
       </c>
+      <c r="C32" s="5">
+        <v>7</v>
+      </c>
       <c r="D32" s="9" t="s">
-        <v>109</v>
-      </c>
-      <c r="F32" s="32">
-        <v>100</v>
-      </c>
-      <c r="G32" s="31">
-        <v>68</v>
-      </c>
-      <c r="H32" s="31">
-        <v>56</v>
-      </c>
-      <c r="I32" s="35">
-        <v>0</v>
-      </c>
-      <c r="J32" s="40">
-        <f t="shared" si="0"/>
-        <v>224</v>
-      </c>
-      <c r="K32" s="38">
-        <v>3</v>
+        <v>30</v>
+      </c>
+      <c r="E32" s="11" t="s">
+        <v>21</v>
+      </c>
+      <c r="F32" s="29">
+        <v>95</v>
+      </c>
+      <c r="G32" s="30">
+        <v>75</v>
+      </c>
+      <c r="H32" s="30">
+        <v>75</v>
+      </c>
+      <c r="I32" s="34">
+        <v>0</v>
+      </c>
+      <c r="J32" s="39">
+        <f>SUM(F32:I32)</f>
+        <v>245</v>
+      </c>
+      <c r="K32" s="37">
+        <v>4</v>
+      </c>
+      <c r="L32" s="25">
+        <v>4</v>
+      </c>
+      <c r="M32" s="1" t="s">
+        <v>40</v>
       </c>
     </row>
     <row r="33" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A33" s="3" t="s">
-        <v>112</v>
+        <v>76</v>
       </c>
       <c r="B33" s="7">
         <v>44441</v>
       </c>
       <c r="C33" s="5">
-        <v>2</v>
+        <v>7</v>
       </c>
       <c r="D33" s="9" t="s">
-        <v>113</v>
-      </c>
-      <c r="E33" s="14" t="s">
-        <v>114</v>
-      </c>
-      <c r="F33" s="32">
-        <v>98</v>
-      </c>
-      <c r="G33" s="31">
-        <v>69</v>
-      </c>
-      <c r="H33" s="31">
+        <v>64</v>
+      </c>
+      <c r="E33" s="11" t="s">
+        <v>77</v>
+      </c>
+      <c r="F33" s="31">
+        <v>101</v>
+      </c>
+      <c r="G33" s="30">
+        <v>64</v>
+      </c>
+      <c r="H33" s="30">
         <v>49</v>
       </c>
-      <c r="I33" s="35">
-        <v>0</v>
-      </c>
-      <c r="J33" s="40">
-        <f t="shared" si="0"/>
-        <v>216</v>
-      </c>
-      <c r="K33" s="38">
+      <c r="I33" s="34">
+        <v>0</v>
+      </c>
+      <c r="J33" s="39">
+        <f>SUM(F33:I33)</f>
+        <v>214</v>
+      </c>
+      <c r="K33" s="37">
         <v>4</v>
       </c>
       <c r="L33" s="26">
         <v>3</v>
       </c>
+      <c r="M33" s="1" t="s">
+        <v>80</v>
+      </c>
     </row>
     <row r="34" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A34" s="3" t="s">
-        <v>115</v>
+        <v>91</v>
       </c>
       <c r="B34" s="7">
         <v>44441</v>
       </c>
       <c r="C34" s="5">
-        <v>-3</v>
+        <v>7</v>
       </c>
       <c r="D34" s="9" t="s">
-        <v>116</v>
+        <v>92</v>
       </c>
       <c r="E34" s="11" t="s">
-        <v>125</v>
-      </c>
-      <c r="F34" s="32">
-        <v>95</v>
-      </c>
-      <c r="G34" s="31">
-        <v>75</v>
-      </c>
-      <c r="H34" s="31">
-        <v>47</v>
-      </c>
-      <c r="I34" s="35">
-        <v>0</v>
-      </c>
-      <c r="J34" s="40">
-        <f t="shared" si="0"/>
-        <v>217</v>
-      </c>
-      <c r="K34" s="38">
+        <v>93</v>
+      </c>
+      <c r="F34" s="31">
+        <v>98</v>
+      </c>
+      <c r="G34" s="30">
+        <v>63</v>
+      </c>
+      <c r="H34" s="30">
+        <v>0</v>
+      </c>
+      <c r="I34" s="34">
+        <v>0</v>
+      </c>
+      <c r="J34" s="39">
+        <f>SUM(F34:I34)</f>
+        <v>161</v>
+      </c>
+      <c r="K34" s="37">
         <v>4</v>
       </c>
       <c r="L34" s="26">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="35" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A35" s="3" t="s">
-        <v>117</v>
+        <v>99</v>
       </c>
       <c r="B35" s="7">
         <v>44441</v>
       </c>
       <c r="C35" s="5">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="D35" s="9" t="s">
-        <v>118</v>
-      </c>
-      <c r="E35" s="11" t="s">
-        <v>119</v>
-      </c>
-      <c r="F35" s="32">
+        <v>101</v>
+      </c>
+      <c r="E35" s="14" t="s">
         <v>100</v>
       </c>
-      <c r="G35" s="31">
-        <v>64</v>
-      </c>
-      <c r="H35" s="31">
-        <v>56</v>
-      </c>
-      <c r="I35" s="35">
-        <v>0</v>
-      </c>
-      <c r="J35" s="40">
-        <f t="shared" si="0"/>
-        <v>220</v>
-      </c>
-      <c r="K35" s="38">
+      <c r="F35" s="31">
+        <v>87</v>
+      </c>
+      <c r="G35" s="30">
+        <v>65</v>
+      </c>
+      <c r="H35" s="30">
+        <v>48</v>
+      </c>
+      <c r="I35" s="34">
+        <v>0</v>
+      </c>
+      <c r="J35" s="39">
+        <f>SUM(F35:I35)</f>
+        <v>200</v>
+      </c>
+      <c r="K35" s="37">
         <v>4</v>
       </c>
       <c r="L35" s="26">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="36" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A36" s="3" t="s">
-        <v>120</v>
+        <v>105</v>
       </c>
       <c r="B36" s="7">
         <v>44441</v>
       </c>
       <c r="C36" s="5">
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="D36" s="9" t="s">
-        <v>121</v>
+        <v>106</v>
       </c>
       <c r="E36" s="11" t="s">
-        <v>122</v>
-      </c>
-      <c r="F36" s="32">
-        <v>91</v>
-      </c>
-      <c r="G36" s="31">
-        <v>51</v>
-      </c>
-      <c r="H36" s="31">
-        <v>33</v>
-      </c>
-      <c r="I36" s="35">
-        <v>0</v>
-      </c>
-      <c r="J36" s="40">
-        <f t="shared" si="0"/>
-        <v>175</v>
-      </c>
-      <c r="K36" s="38">
+        <v>93</v>
+      </c>
+      <c r="F36" s="31">
+        <v>98</v>
+      </c>
+      <c r="G36" s="30">
+        <v>66</v>
+      </c>
+      <c r="H36" s="30">
+        <v>58</v>
+      </c>
+      <c r="I36" s="34">
+        <v>0</v>
+      </c>
+      <c r="J36" s="39">
+        <f>SUM(F36:I36)</f>
+        <v>222</v>
+      </c>
+      <c r="K36" s="37">
         <v>4</v>
       </c>
       <c r="L36" s="26">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="37" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A37" s="3" t="s">
-        <v>123</v>
+        <v>144</v>
       </c>
       <c r="B37" s="7">
         <v>44442</v>
       </c>
       <c r="C37" s="5">
-        <v>2</v>
+        <v>7</v>
       </c>
       <c r="D37" s="9" t="s">
-        <v>29</v>
-      </c>
-      <c r="E37" s="14" t="s">
-        <v>124</v>
-      </c>
-      <c r="F37" s="32">
-        <v>99</v>
-      </c>
-      <c r="G37" s="31">
-        <v>82</v>
-      </c>
-      <c r="H37" s="31">
-        <v>55</v>
-      </c>
-      <c r="I37" s="35">
-        <v>0</v>
-      </c>
-      <c r="J37" s="40">
-        <f t="shared" si="0"/>
-        <v>236</v>
-      </c>
-      <c r="K37" s="38">
-        <v>5</v>
+        <v>145</v>
+      </c>
+      <c r="F37" s="31">
+        <v>98</v>
+      </c>
+      <c r="G37" s="30">
+        <v>66</v>
+      </c>
+      <c r="H37" s="30">
+        <v>49</v>
+      </c>
+      <c r="I37" s="34">
+        <v>0</v>
+      </c>
+      <c r="J37" s="39">
+        <f>SUM(F37:I37)</f>
+        <v>213</v>
+      </c>
+      <c r="K37" s="37">
+        <v>4</v>
       </c>
       <c r="L37" s="26">
         <v>4</v>
-      </c>
-      <c r="M37" s="1" t="s">
-        <v>39</v>
       </c>
     </row>
     <row r="38" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A38" s="3" t="s">
-        <v>127</v>
+        <v>147</v>
       </c>
       <c r="B38" s="7">
         <v>44442</v>
       </c>
       <c r="C38" s="5">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="D38" s="9" t="s">
-        <v>128</v>
-      </c>
-      <c r="E38" s="11" t="s">
-        <v>122</v>
-      </c>
-      <c r="F38" s="32">
-        <v>100</v>
-      </c>
-      <c r="G38" s="31">
-        <v>68</v>
-      </c>
-      <c r="H38" s="31">
-        <v>50</v>
-      </c>
-      <c r="I38" s="35">
-        <v>0</v>
-      </c>
-      <c r="J38" s="40">
-        <f t="shared" si="0"/>
-        <v>218</v>
-      </c>
-      <c r="K38" s="38">
+        <v>152</v>
+      </c>
+      <c r="E38" s="14" t="s">
+        <v>154</v>
+      </c>
+      <c r="F38" s="31">
+        <v>95</v>
+      </c>
+      <c r="G38" s="30">
+        <v>63</v>
+      </c>
+      <c r="H38" s="30">
+        <v>45</v>
+      </c>
+      <c r="I38" s="34">
+        <v>0</v>
+      </c>
+      <c r="J38" s="39">
+        <f>SUM(F38:I38)</f>
+        <v>203</v>
+      </c>
+      <c r="K38" s="37">
         <v>4</v>
       </c>
       <c r="L38" s="26">
         <v>3</v>
       </c>
-      <c r="M38" s="1" t="s">
-        <v>129</v>
-      </c>
     </row>
     <row r="39" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A39" s="3" t="s">
-        <v>130</v>
+        <v>10</v>
       </c>
       <c r="B39" s="7">
-        <v>44442</v>
+        <v>44441</v>
       </c>
       <c r="C39" s="5">
-        <v>1</v>
+        <v>8</v>
       </c>
       <c r="D39" s="9" t="s">
-        <v>131</v>
+        <v>56</v>
       </c>
       <c r="E39" s="11" t="s">
-        <v>132</v>
-      </c>
-      <c r="F39" s="32">
-        <v>155</v>
-      </c>
-      <c r="G39" s="31">
+        <v>57</v>
+      </c>
+      <c r="F39" s="29">
         <v>98</v>
       </c>
-      <c r="H39" s="31">
-        <v>93</v>
-      </c>
-      <c r="I39" s="35">
-        <v>0</v>
-      </c>
-      <c r="J39" s="40">
-        <f t="shared" si="0"/>
-        <v>346</v>
-      </c>
-      <c r="K39" s="38">
-        <v>5</v>
-      </c>
-      <c r="L39" s="26">
-        <v>4</v>
+      <c r="G39" s="30">
+        <v>72</v>
+      </c>
+      <c r="H39" s="30">
+        <v>53</v>
+      </c>
+      <c r="I39" s="34">
+        <v>0</v>
+      </c>
+      <c r="J39" s="39">
+        <f>SUM(F39:I39)</f>
+        <v>223</v>
+      </c>
+      <c r="K39" s="37">
+        <v>4</v>
+      </c>
+      <c r="L39" s="25">
+        <v>3</v>
+      </c>
+      <c r="M39" s="1" t="s">
+        <v>58</v>
       </c>
     </row>
     <row r="40" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A40" s="3" t="s">
-        <v>133</v>
+        <v>25</v>
       </c>
       <c r="B40" s="7">
-        <v>44442</v>
+        <v>44441</v>
       </c>
       <c r="C40" s="5">
-        <v>1</v>
+        <v>8</v>
       </c>
       <c r="D40" s="9" t="s">
-        <v>134</v>
+        <v>27</v>
       </c>
       <c r="E40" s="11" t="s">
-        <v>135</v>
-      </c>
-      <c r="F40" s="32">
-        <v>69</v>
-      </c>
-      <c r="G40" s="31">
-        <v>68</v>
-      </c>
-      <c r="H40" s="31">
-        <v>45</v>
-      </c>
-      <c r="I40" s="35">
-        <v>0</v>
-      </c>
-      <c r="J40" s="40">
-        <f t="shared" si="0"/>
-        <v>182</v>
+        <v>26</v>
+      </c>
+      <c r="F40" s="31">
+        <v>95</v>
+      </c>
+      <c r="G40" s="30">
+        <v>74</v>
+      </c>
+      <c r="H40" s="30">
+        <v>54</v>
+      </c>
+      <c r="I40" s="34">
+        <v>0</v>
+      </c>
+      <c r="J40" s="39">
+        <f>SUM(F40:I40)</f>
+        <v>223</v>
+      </c>
+      <c r="K40" s="37">
+        <v>4</v>
       </c>
       <c r="L40" s="26">
-        <v>2</v>
-      </c>
-      <c r="M40" s="1" t="s">
-        <v>136</v>
+        <v>3</v>
       </c>
     </row>
     <row r="41" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A41" s="3" t="s">
-        <v>164</v>
+        <v>36</v>
+      </c>
+      <c r="B41" s="7">
+        <v>44441</v>
+      </c>
+      <c r="C41" s="5">
+        <v>8</v>
+      </c>
+      <c r="D41" s="9" t="s">
+        <v>37</v>
+      </c>
+      <c r="E41" s="11" t="s">
+        <v>38</v>
+      </c>
+      <c r="F41" s="31">
+        <v>97</v>
+      </c>
+      <c r="G41" s="30">
+        <v>71</v>
+      </c>
+      <c r="H41" s="30">
+        <v>54</v>
+      </c>
+      <c r="I41" s="34">
+        <v>0</v>
+      </c>
+      <c r="J41" s="39">
+        <f>SUM(F41:I41)</f>
+        <v>222</v>
+      </c>
+      <c r="K41" s="37">
+        <v>4</v>
+      </c>
+      <c r="L41" s="26">
+        <v>4</v>
+      </c>
+      <c r="M41" s="1" t="s">
+        <v>39</v>
       </c>
     </row>
     <row r="42" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A42" s="3" t="s">
-        <v>137</v>
+        <v>87</v>
       </c>
       <c r="B42" s="7">
-        <v>44442</v>
+        <v>44441</v>
       </c>
       <c r="C42" s="5">
-        <v>1</v>
+        <v>8</v>
       </c>
       <c r="D42" s="9" t="s">
-        <v>138</v>
+        <v>88</v>
       </c>
       <c r="E42" s="11" t="s">
-        <v>139</v>
-      </c>
-      <c r="F42" s="32">
-        <v>112</v>
-      </c>
-      <c r="G42" s="31">
-        <v>86</v>
-      </c>
-      <c r="H42" s="31">
-        <v>51</v>
-      </c>
-      <c r="I42" s="35">
-        <v>0</v>
-      </c>
-      <c r="J42" s="40">
-        <f t="shared" si="0"/>
-        <v>249</v>
-      </c>
-      <c r="K42" s="38">
-        <v>5</v>
+        <v>89</v>
+      </c>
+      <c r="F42" s="31">
+        <v>72</v>
+      </c>
+      <c r="G42" s="30">
+        <v>55</v>
+      </c>
+      <c r="H42" s="30">
+        <v>39</v>
+      </c>
+      <c r="I42" s="34">
+        <v>0</v>
+      </c>
+      <c r="J42" s="39">
+        <f>SUM(F42:I42)</f>
+        <v>166</v>
+      </c>
+      <c r="K42" s="37">
+        <v>4</v>
       </c>
       <c r="L42" s="26">
         <v>3</v>
       </c>
+      <c r="M42" s="1" t="s">
+        <v>90</v>
+      </c>
     </row>
     <row r="43" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A43" s="3" t="s">
-        <v>140</v>
+        <v>146</v>
+      </c>
+      <c r="B43" s="7">
+        <v>44442</v>
+      </c>
+      <c r="C43" s="5">
+        <v>8</v>
       </c>
       <c r="D43" s="9" t="s">
-        <v>161</v>
-      </c>
-      <c r="J43" s="40">
-        <f t="shared" si="0"/>
-        <v>0</v>
+        <v>150</v>
+      </c>
+      <c r="F43" s="31">
+        <v>96</v>
+      </c>
+      <c r="G43" s="30">
+        <v>53</v>
+      </c>
+      <c r="H43" s="30">
+        <v>49</v>
+      </c>
+      <c r="I43" s="34">
+        <v>0</v>
+      </c>
+      <c r="J43" s="39">
+        <f>SUM(F43:I43)</f>
+        <v>198</v>
+      </c>
+      <c r="K43" s="37">
+        <v>4</v>
+      </c>
+      <c r="L43" s="26">
+        <v>3</v>
       </c>
       <c r="M43" s="1" t="s">
-        <v>141</v>
+        <v>151</v>
       </c>
     </row>
     <row r="44" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A44" s="3" t="s">
-        <v>142</v>
+        <v>155</v>
       </c>
       <c r="B44" s="7">
         <v>44442</v>
       </c>
       <c r="C44" s="5">
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="D44" s="9" t="s">
-        <v>143</v>
-      </c>
-      <c r="F44" s="32">
-        <v>49</v>
-      </c>
-      <c r="G44" s="31">
         <v>32</v>
       </c>
-      <c r="H44" s="31">
-        <v>0</v>
-      </c>
-      <c r="I44" s="35">
-        <v>0</v>
-      </c>
-      <c r="J44" s="40">
-        <f t="shared" si="0"/>
-        <v>81</v>
-      </c>
-      <c r="K44" s="38">
-        <v>3</v>
+      <c r="E44" s="11" t="s">
+        <v>22</v>
+      </c>
+      <c r="F44" s="31">
+        <v>97</v>
+      </c>
+      <c r="G44" s="30">
+        <v>64</v>
+      </c>
+      <c r="H44" s="30">
+        <v>36</v>
+      </c>
+      <c r="I44" s="34">
+        <v>0</v>
+      </c>
+      <c r="J44" s="39">
+        <f>SUM(F44:I44)</f>
+        <v>197</v>
+      </c>
+      <c r="K44" s="37">
+        <v>4</v>
       </c>
       <c r="L44" s="26">
         <v>3</v>
       </c>
-      <c r="M44" s="1" t="s">
-        <v>39</v>
-      </c>
     </row>
     <row r="45" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A45" s="3" t="s">
-        <v>145</v>
+        <v>156</v>
       </c>
       <c r="B45" s="7">
         <v>44442</v>
       </c>
       <c r="C45" s="5">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="D45" s="9" t="s">
-        <v>146</v>
-      </c>
-      <c r="F45" s="32">
-        <v>98</v>
-      </c>
-      <c r="G45" s="31">
-        <v>66</v>
-      </c>
-      <c r="H45" s="31">
-        <v>49</v>
-      </c>
-      <c r="I45" s="35">
-        <v>0</v>
-      </c>
-      <c r="J45" s="40">
-        <f t="shared" si="0"/>
-        <v>213</v>
-      </c>
-      <c r="K45" s="38">
+        <v>32</v>
+      </c>
+      <c r="E45" s="11" t="s">
+        <v>22</v>
+      </c>
+      <c r="F45" s="31">
+        <v>122</v>
+      </c>
+      <c r="G45" s="30">
+        <v>91</v>
+      </c>
+      <c r="H45" s="30">
+        <v>89</v>
+      </c>
+      <c r="I45" s="34">
+        <v>0</v>
+      </c>
+      <c r="J45" s="39">
+        <f>SUM(F45:I45)</f>
+        <v>302</v>
+      </c>
+      <c r="K45" s="37">
         <v>4</v>
       </c>
       <c r="L45" s="26">
@@ -3079,290 +3378,250 @@
     </row>
     <row r="46" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A46" s="3" t="s">
-        <v>147</v>
+        <v>161</v>
       </c>
       <c r="B46" s="7">
-        <v>44442</v>
+        <v>44443</v>
       </c>
       <c r="C46" s="5">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="D46" s="9" t="s">
-        <v>151</v>
-      </c>
-      <c r="F46" s="32">
-        <v>96</v>
-      </c>
-      <c r="G46" s="31">
-        <v>53</v>
-      </c>
-      <c r="H46" s="31">
-        <v>49</v>
-      </c>
-      <c r="I46" s="35">
-        <v>0</v>
-      </c>
-      <c r="J46" s="40">
-        <f t="shared" si="0"/>
-        <v>198</v>
-      </c>
-      <c r="K46" s="38">
-        <v>4</v>
+        <v>162</v>
+      </c>
+      <c r="E46" s="11" t="s">
+        <v>162</v>
+      </c>
+      <c r="F46" s="31">
+        <v>122</v>
+      </c>
+      <c r="G46" s="30">
+        <v>75</v>
+      </c>
+      <c r="H46" s="30">
+        <v>55</v>
+      </c>
+      <c r="I46" s="34">
+        <v>0</v>
+      </c>
+      <c r="J46" s="39">
+        <f>SUM(F46:I46)</f>
+        <v>252</v>
+      </c>
+      <c r="K46" s="37">
+        <v>5</v>
       </c>
       <c r="L46" s="26">
         <v>3</v>
       </c>
-      <c r="M46" s="1" t="s">
-        <v>152</v>
-      </c>
     </row>
     <row r="47" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A47" s="3" t="s">
-        <v>149</v>
+        <v>12</v>
       </c>
       <c r="B47" s="7">
-        <v>44442</v>
-      </c>
-      <c r="M47" s="1" t="s">
-        <v>154</v>
+        <v>44441</v>
+      </c>
+      <c r="C47" s="5">
+        <v>10</v>
+      </c>
+      <c r="D47" s="9" t="s">
+        <v>29</v>
+      </c>
+      <c r="E47" s="11" t="s">
+        <v>23</v>
+      </c>
+      <c r="F47" s="29">
+        <v>100</v>
+      </c>
+      <c r="G47" s="30">
+        <v>70</v>
+      </c>
+      <c r="H47" s="30">
+        <v>50</v>
+      </c>
+      <c r="I47" s="34">
+        <v>0</v>
+      </c>
+      <c r="J47" s="39">
+        <f>SUM(F47:I47)</f>
+        <v>220</v>
+      </c>
+      <c r="K47" s="37">
+        <v>4</v>
+      </c>
+      <c r="L47" s="25">
+        <v>4</v>
       </c>
     </row>
     <row r="48" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A48" s="3" t="s">
+        <v>110</v>
+      </c>
+      <c r="B48" s="7">
+        <v>44441</v>
+      </c>
+      <c r="D48" s="9" t="s">
+        <v>109</v>
+      </c>
+      <c r="F48" s="31">
+        <v>100</v>
+      </c>
+      <c r="G48" s="30">
+        <v>68</v>
+      </c>
+      <c r="H48" s="30">
+        <v>56</v>
+      </c>
+      <c r="I48" s="34">
+        <v>0</v>
+      </c>
+      <c r="J48" s="39">
+        <f>SUM(F48:I48)</f>
+        <v>224</v>
+      </c>
+      <c r="K48" s="37">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="49" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A49" s="3" t="s">
+        <v>140</v>
+      </c>
+      <c r="D49" s="9" t="s">
+        <v>160</v>
+      </c>
+      <c r="J49" s="39">
+        <f>SUM(F49:I49)</f>
+        <v>0</v>
+      </c>
+      <c r="M49" s="1" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="50" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A50" s="3" t="s">
         <v>148</v>
-      </c>
-      <c r="B48" s="7">
-        <v>44442</v>
-      </c>
-      <c r="C48" s="5">
-        <v>7</v>
-      </c>
-      <c r="D48" s="9" t="s">
-        <v>153</v>
-      </c>
-      <c r="E48" s="14" t="s">
-        <v>155</v>
-      </c>
-      <c r="F48" s="32">
-        <v>95</v>
-      </c>
-      <c r="G48" s="31">
-        <v>63</v>
-      </c>
-      <c r="H48" s="31">
-        <v>45</v>
-      </c>
-      <c r="I48" s="35">
-        <v>0</v>
-      </c>
-      <c r="J48" s="40">
-        <f>SUM(F48:I48)</f>
-        <v>203</v>
-      </c>
-      <c r="K48" s="38">
-        <v>4</v>
-      </c>
-      <c r="L48" s="26">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="49" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A49" s="3" t="s">
-        <v>156</v>
-      </c>
-      <c r="B49" s="7">
-        <v>44442</v>
-      </c>
-      <c r="C49" s="5">
-        <v>8</v>
-      </c>
-      <c r="D49" s="9" t="s">
-        <v>32</v>
-      </c>
-      <c r="E49" s="11" t="s">
-        <v>22</v>
-      </c>
-      <c r="F49" s="32">
-        <v>97</v>
-      </c>
-      <c r="G49" s="31">
-        <v>64</v>
-      </c>
-      <c r="H49" s="31">
-        <v>36</v>
-      </c>
-      <c r="I49" s="35">
-        <v>0</v>
-      </c>
-      <c r="J49" s="40">
-        <f>SUM(F49:I49)</f>
-        <v>197</v>
-      </c>
-      <c r="K49" s="38">
-        <v>4</v>
-      </c>
-      <c r="L49" s="26">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="50" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A50" s="3" t="s">
-        <v>157</v>
       </c>
       <c r="B50" s="7">
         <v>44442</v>
       </c>
-      <c r="C50" s="5">
-        <v>8</v>
-      </c>
-      <c r="D50" s="9" t="s">
-        <v>32</v>
-      </c>
-      <c r="E50" s="11" t="s">
-        <v>22</v>
-      </c>
-      <c r="F50" s="32">
-        <v>122</v>
-      </c>
-      <c r="G50" s="31">
-        <v>91</v>
-      </c>
-      <c r="H50" s="31">
-        <v>89</v>
-      </c>
-      <c r="I50" s="35">
-        <v>0</v>
-      </c>
-      <c r="J50" s="40">
-        <f>SUM(F50:I50)</f>
-        <v>302</v>
-      </c>
-      <c r="K50" s="38">
-        <v>4</v>
-      </c>
-      <c r="L50" s="26">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="51" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M50" s="1" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="51" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A51" s="3" t="s">
+        <v>157</v>
+      </c>
+      <c r="B51" s="7" t="s">
         <v>158</v>
       </c>
-      <c r="B51" s="7" t="s">
+      <c r="D51" s="9" t="s">
         <v>159</v>
       </c>
-      <c r="D51" s="9" t="s">
-        <v>160</v>
-      </c>
-      <c r="J51" s="40">
-        <f t="shared" ref="J51:J52" si="1">SUM(F51:I51)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="52" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="J51" s="39">
+        <f>SUM(F51:I51)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="52" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A52" s="3" t="s">
-        <v>162</v>
-      </c>
-      <c r="B52" s="7">
-        <v>44443</v>
-      </c>
-      <c r="C52" s="5">
-        <v>9</v>
-      </c>
-      <c r="D52" s="9" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="53" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A53" s="3" t="s">
         <v>163</v>
       </c>
-      <c r="E52" s="11" t="s">
-        <v>163</v>
-      </c>
-      <c r="F52" s="32">
-        <v>122</v>
-      </c>
-      <c r="G52" s="31">
-        <v>75</v>
-      </c>
-      <c r="H52" s="31">
-        <v>55</v>
-      </c>
-      <c r="I52" s="35">
-        <v>0</v>
-      </c>
-      <c r="J52" s="40">
-        <f t="shared" si="1"/>
-        <v>252</v>
-      </c>
-      <c r="K52" s="38">
-        <v>5</v>
-      </c>
-      <c r="L52" s="26">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="53" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A53" s="3" t="s">
+    </row>
+    <row r="54" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A54" s="3" t="s">
         <v>165</v>
       </c>
     </row>
-    <row r="54" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A54" s="3" t="s">
-        <v>166</v>
-      </c>
-    </row>
-    <row r="55" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A55" s="3" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="56" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A56" s="3" t="s">
         <v>168</v>
       </c>
     </row>
-    <row r="56" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A56" s="3" t="s">
+    <row r="57" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A57" s="3" t="s">
         <v>169</v>
       </c>
     </row>
-    <row r="57" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A57" s="3" t="s">
+    <row r="58" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A58" s="3" t="s">
         <v>170</v>
       </c>
     </row>
-    <row r="58" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A58" s="3" t="s">
+    <row r="59" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A59" s="3" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="60" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A60" s="3" t="s">
         <v>171</v>
       </c>
     </row>
-    <row r="59" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A59" s="3" t="s">
+    <row r="61" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A61" s="3" t="s">
         <v>172</v>
       </c>
     </row>
-    <row r="60" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A60" s="3" t="s">
+    <row r="62" spans="1:13" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A62" s="43"/>
+      <c r="B62" s="44"/>
+      <c r="C62" s="45"/>
+      <c r="D62" s="46"/>
+      <c r="E62" s="47"/>
+      <c r="F62" s="48"/>
+      <c r="G62" s="49"/>
+      <c r="H62" s="49"/>
+      <c r="I62" s="50"/>
+      <c r="J62" s="51"/>
+      <c r="K62" s="52"/>
+      <c r="L62" s="53"/>
+    </row>
+    <row r="63" spans="1:13" ht="18.600000000000001" thickTop="1" x14ac:dyDescent="0.3">
+      <c r="A63" s="54" t="s">
         <v>173</v>
       </c>
-    </row>
-    <row r="61" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A61" s="3" t="s">
-        <v>174</v>
-      </c>
-    </row>
-    <row r="63" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A63" s="3" t="s">
-        <v>144</v>
-      </c>
-      <c r="B63" s="5">
-        <f>COUNTBLANK(B3:B62)</f>
-        <v>12</v>
-      </c>
+      <c r="B63" s="55">
+        <f xml:space="preserve"> COUNTBLANK(B3:B61) - COUNTBLANK(A3:A61)</f>
+        <v>11</v>
+      </c>
+      <c r="C63" s="4"/>
+      <c r="D63" s="8"/>
+      <c r="E63" s="10"/>
+      <c r="F63" s="42"/>
+      <c r="G63" s="28"/>
+      <c r="H63" s="28"/>
+      <c r="I63" s="33"/>
+      <c r="J63" s="38"/>
+      <c r="K63" s="36"/>
+      <c r="L63" s="24"/>
     </row>
   </sheetData>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A3:M62">
+    <sortCondition ref="C3:C62"/>
+  </sortState>
   <mergeCells count="1">
     <mergeCell ref="F1:I1"/>
   </mergeCells>
-  <conditionalFormatting sqref="L3:L46 L48:L1048576">
-    <cfRule type="cellIs" dxfId="2" priority="7" operator="greaterThan">
+  <conditionalFormatting sqref="L3:L45 L63:L1048576 L47:L61">
+    <cfRule type="cellIs" dxfId="5" priority="8" operator="greaterThan">
       <formula>3</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="K3:K46 K48:K1048576">
-    <cfRule type="colorScale" priority="6">
+  <conditionalFormatting sqref="K3:K45 K63:K1048576 K47:K61">
+    <cfRule type="colorScale" priority="7">
       <colorScale>
         <cfvo type="num" val="2"/>
         <cfvo type="max"/>
@@ -3371,8 +3630,8 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F3:I46 F48:I1048576">
-    <cfRule type="colorScale" priority="5">
+  <conditionalFormatting sqref="F3:I45 F63:I1048576 F47:I61">
+    <cfRule type="colorScale" priority="6">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="max"/>
@@ -3381,8 +3640,8 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C1:C1048576">
-    <cfRule type="colorScale" priority="4">
+  <conditionalFormatting sqref="C63:C1048576 C1:C61">
+    <cfRule type="colorScale" priority="5">
       <colorScale>
         <cfvo type="num" val="-12"/>
         <cfvo type="num" val="0"/>
@@ -3393,11 +3652,8 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A1:A1048576">
-    <cfRule type="duplicateValues" dxfId="1" priority="3"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="J1:J46 J48:J1048576">
-    <cfRule type="colorScale" priority="2">
+  <conditionalFormatting sqref="J1:J45 J63:J1048576 J47:J61">
+    <cfRule type="colorScale" priority="3">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="max"/>
@@ -3406,12 +3662,27 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B1:B1048576">
-    <cfRule type="containsBlanks" dxfId="0" priority="1">
-      <formula>LEN(TRIM(B1))=0</formula>
+  <conditionalFormatting sqref="B3:L62">
+    <cfRule type="containsBlanks" dxfId="4" priority="9">
+      <formula>LEN(TRIM(B3))=0</formula>
     </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A63:A1048576 A1:A61">
+    <cfRule type="duplicateValues" dxfId="3" priority="24"/>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{632A4462-8ECA-4668-A671-4BCBF233D2F6}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>